<commit_message>
Added units to graphs
</commit_message>
<xml_diff>
--- a/project2/documents/result-data.xlsx
+++ b/project2/documents/result-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sarah\college\sysnetI\project2\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145B4132-4B99-4936-96FE-1AB5588C82EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5385C14D-729E-4C9D-9738-17BE383FB2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3D1A821C-EF8D-427E-966F-71BAC62ACC95}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{3D1A821C-EF8D-427E-966F-71BAC62ACC95}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="7" r:id="rId1"/>
@@ -20,8 +20,6 @@
     <definedName name="_xlchart.v1.0" hidden="1">results!$C$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">results!$C$2:$C$438</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">results!$A$2:$A$438</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">results!$C$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">results!$C$2:$C$438</definedName>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">times!$B$2:$B$12</definedName>
     <definedName name="ExternalData_2" localSheetId="0" hidden="1">results!$A$1:$B$438</definedName>
   </definedNames>
@@ -455,12 +453,6 @@
     <t>Average</t>
   </si>
   <si>
-    <t>Measured Times w/ Lock</t>
-  </si>
-  <si>
-    <t>Measured Times w/o Lock</t>
-  </si>
-  <si>
     <t>Run 1</t>
   </si>
   <si>
@@ -1182,6 +1174,12 @@
   </si>
   <si>
     <t>Frequency Values</t>
+  </si>
+  <si>
+    <t>Measured Times w/ Lock in Seconds</t>
+  </si>
+  <si>
+    <t>Measured Times w/o Lock in Seconds</t>
   </si>
 </sst>
 </file>
@@ -1313,7 +1311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1325,22 +1323,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1404,6 +1395,12 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1739,7 +1736,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Time</a:t>
+                  <a:t> Time (s)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2185,7 +2182,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Time</a:t>
+                  <a:t> Time (s)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -4923,8 +4920,8 @@
   <autoFilter ref="A1:C438" xr:uid="{F50FCF36-CE9B-444C-A0D7-F6EB36CDACD6}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7034E7C0-4369-40D2-B3AD-986C8D7D784C}" uniqueName="1" name="Stopping times" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{B608315C-71DF-4745-8408-3A01CAD04511}" uniqueName="2" name="Stopping times frequency" queryTableFieldId="2" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{D48065B0-154E-4711-8807-300D11819B0D}" uniqueName="3" name="Frequency Values" queryTableFieldId="3" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{B608315C-71DF-4745-8408-3A01CAD04511}" uniqueName="2" name="Stopping times frequency" queryTableFieldId="2" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{D48065B0-154E-4711-8807-300D11819B0D}" uniqueName="3" name="Frequency Values" queryTableFieldId="3" dataDxfId="8">
       <calculatedColumnFormula>VALUE(MID(B2, FIND("(", B2) + 1, FIND(")", B2) - FIND("(", B2) - 1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4936,28 +4933,28 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BDC70456-C47D-4E86-A88C-DA389D492E4D}" name="results__4" displayName="results__4" ref="B2:I13" tableType="queryTable" totalsRowCount="1">
   <autoFilter ref="B2:I12" xr:uid="{BDC70456-C47D-4E86-A88C-DA389D492E4D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{35AB05AD-C427-4434-A913-0EDA89286862}" uniqueName="1" name="1 Thread" totalsRowFunction="custom" queryTableFieldId="1" totalsRowDxfId="9">
+    <tableColumn id="1" xr3:uid="{35AB05AD-C427-4434-A913-0EDA89286862}" uniqueName="1" name="1 Thread" totalsRowFunction="custom" queryTableFieldId="1" totalsRowDxfId="7">
       <totalsRowFormula>AVERAGE(results__4[1 Thread])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{0CF63B9C-D520-40CF-A961-0A06E0808F0F}" uniqueName="2" name="2 Threads" totalsRowFunction="custom" queryTableFieldId="2" totalsRowDxfId="8">
+    <tableColumn id="2" xr3:uid="{0CF63B9C-D520-40CF-A961-0A06E0808F0F}" uniqueName="2" name="2 Threads" totalsRowFunction="custom" queryTableFieldId="2" totalsRowDxfId="6">
       <totalsRowFormula>AVERAGE(results__4[2 Threads])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{560E26C1-6A70-4010-B1D0-84F87CB54313}" uniqueName="3" name="3 Threads" totalsRowFunction="custom" queryTableFieldId="3" totalsRowDxfId="7">
+    <tableColumn id="3" xr3:uid="{560E26C1-6A70-4010-B1D0-84F87CB54313}" uniqueName="3" name="3 Threads" totalsRowFunction="custom" queryTableFieldId="3" totalsRowDxfId="5">
       <totalsRowFormula>AVERAGE(results__4[3 Threads])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C3229C64-1100-42F0-B6C2-8C86FD806630}" uniqueName="4" name="4 Threads" totalsRowFunction="custom" queryTableFieldId="4" totalsRowDxfId="6">
+    <tableColumn id="4" xr3:uid="{C3229C64-1100-42F0-B6C2-8C86FD806630}" uniqueName="4" name="4 Threads" totalsRowFunction="custom" queryTableFieldId="4" totalsRowDxfId="4">
       <totalsRowFormula>AVERAGE(results__4[4 Threads])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5D2EE9E6-75E2-47FB-8EEB-56385E0E823F}" uniqueName="5" name="5 Threads" totalsRowFunction="custom" queryTableFieldId="5" totalsRowDxfId="5">
+    <tableColumn id="5" xr3:uid="{5D2EE9E6-75E2-47FB-8EEB-56385E0E823F}" uniqueName="5" name="5 Threads" totalsRowFunction="custom" queryTableFieldId="5" totalsRowDxfId="3">
       <totalsRowFormula>AVERAGE(results__4[5 Threads])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{58FA579E-54BF-4CE2-B251-7CBEF6C83D4B}" uniqueName="6" name="6 Threads" totalsRowFunction="custom" queryTableFieldId="6" totalsRowDxfId="4">
+    <tableColumn id="6" xr3:uid="{58FA579E-54BF-4CE2-B251-7CBEF6C83D4B}" uniqueName="6" name="6 Threads" totalsRowFunction="custom" queryTableFieldId="6" totalsRowDxfId="2">
       <totalsRowFormula>AVERAGE(results__4[6 Threads])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{81270D10-1438-48A0-93B0-A3751A05598C}" uniqueName="7" name="7 Threads" totalsRowFunction="custom" queryTableFieldId="7" totalsRowDxfId="3">
+    <tableColumn id="7" xr3:uid="{81270D10-1438-48A0-93B0-A3751A05598C}" uniqueName="7" name="7 Threads" totalsRowFunction="custom" queryTableFieldId="7" totalsRowDxfId="1">
       <totalsRowFormula>AVERAGE(results__4[7 Threads])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{44530E4E-18B9-4218-828F-B0AA3F001A0C}" uniqueName="8" name="8 Threads" totalsRowFunction="custom" queryTableFieldId="8" totalsRowDxfId="2">
+    <tableColumn id="8" xr3:uid="{44530E4E-18B9-4218-828F-B0AA3F001A0C}" uniqueName="8" name="8 Threads" totalsRowFunction="custom" queryTableFieldId="8" totalsRowDxfId="0">
       <totalsRowFormula>AVERAGE(results__4[8 Threads])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -5284,7 +5281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61468CB4-8593-4B47-9373-3CCC2C3AA5A5}">
   <dimension ref="A1:D438"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
@@ -5303,7 +5300,7 @@
         <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>107</v>
@@ -5313,14 +5310,14 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C65" si="0">VALUE(MID(B2, FIND("(", B2) + 1, FIND(")", B2) - FIND("(", B2) - 1))</f>
         <v>1</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="11">
         <v>1000000</v>
       </c>
     </row>
@@ -5328,7 +5325,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3">
@@ -5340,7 +5337,7 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4">
@@ -5352,7 +5349,7 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5">
@@ -5364,7 +5361,7 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6">
@@ -5376,7 +5373,7 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7">
@@ -5388,7 +5385,7 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8">
@@ -5400,7 +5397,7 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9">
@@ -5412,7 +5409,7 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10">
@@ -5424,7 +5421,7 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11">
@@ -5436,7 +5433,7 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12">
@@ -5448,7 +5445,7 @@
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13">
@@ -5460,7 +5457,7 @@
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14">
@@ -5472,7 +5469,7 @@
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15">
@@ -5484,7 +5481,7 @@
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
@@ -5496,7 +5493,7 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" t="s">
         <v>21</v>
       </c>
       <c r="C17">
@@ -5508,7 +5505,7 @@
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" t="s">
         <v>23</v>
       </c>
       <c r="C18">
@@ -5520,7 +5517,7 @@
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" t="s">
         <v>29</v>
       </c>
       <c r="C19">
@@ -5532,7 +5529,7 @@
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" t="s">
         <v>33</v>
       </c>
       <c r="C20">
@@ -5544,7 +5541,7 @@
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" t="s">
         <v>39</v>
       </c>
       <c r="C21">
@@ -5556,7 +5553,7 @@
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" t="s">
         <v>44</v>
       </c>
       <c r="C22">
@@ -5568,7 +5565,7 @@
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" t="s">
         <v>49</v>
       </c>
       <c r="C23">
@@ -5580,7 +5577,7 @@
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" t="s">
         <v>59</v>
       </c>
       <c r="C24">
@@ -5592,7 +5589,7 @@
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" t="s">
         <v>62</v>
       </c>
       <c r="C25">
@@ -5604,7 +5601,7 @@
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" t="s">
         <v>71</v>
       </c>
       <c r="C26">
@@ -5616,7 +5613,7 @@
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" t="s">
         <v>78</v>
       </c>
       <c r="C27">
@@ -5628,7 +5625,7 @@
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" t="s">
         <v>83</v>
       </c>
       <c r="C28">
@@ -5640,7 +5637,7 @@
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" t="s">
         <v>92</v>
       </c>
       <c r="C29">
@@ -5652,7 +5649,7 @@
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" t="s">
         <v>93</v>
       </c>
       <c r="C30">
@@ -5664,7 +5661,7 @@
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" t="s">
         <v>102</v>
       </c>
       <c r="C31">
@@ -5676,8 +5673,8 @@
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>129</v>
+      <c r="B32" t="s">
+        <v>127</v>
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
@@ -5688,8 +5685,8 @@
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>130</v>
+      <c r="B33" t="s">
+        <v>128</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
@@ -5700,8 +5697,8 @@
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>131</v>
+      <c r="B34" t="s">
+        <v>129</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
@@ -5712,8 +5709,8 @@
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>132</v>
+      <c r="B35" t="s">
+        <v>130</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
@@ -5724,8 +5721,8 @@
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>133</v>
+      <c r="B36" t="s">
+        <v>131</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
@@ -5736,8 +5733,8 @@
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" s="12" t="s">
-        <v>134</v>
+      <c r="B37" t="s">
+        <v>132</v>
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
@@ -5748,8 +5745,8 @@
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" s="12" t="s">
-        <v>135</v>
+      <c r="B38" t="s">
+        <v>133</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
@@ -5760,8 +5757,8 @@
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>136</v>
+      <c r="B39" t="s">
+        <v>134</v>
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
@@ -5772,8 +5769,8 @@
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" s="12" t="s">
-        <v>137</v>
+      <c r="B40" t="s">
+        <v>135</v>
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
@@ -5784,8 +5781,8 @@
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>138</v>
+      <c r="B41" t="s">
+        <v>136</v>
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
@@ -5796,8 +5793,8 @@
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>139</v>
+      <c r="B42" t="s">
+        <v>137</v>
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
@@ -5808,8 +5805,8 @@
       <c r="A43">
         <v>41</v>
       </c>
-      <c r="B43" s="12" t="s">
-        <v>140</v>
+      <c r="B43" t="s">
+        <v>138</v>
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
@@ -5820,8 +5817,8 @@
       <c r="A44">
         <v>42</v>
       </c>
-      <c r="B44" s="12" t="s">
-        <v>141</v>
+      <c r="B44" t="s">
+        <v>139</v>
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
@@ -5832,8 +5829,8 @@
       <c r="A45">
         <v>43</v>
       </c>
-      <c r="B45" s="12" t="s">
-        <v>142</v>
+      <c r="B45" t="s">
+        <v>140</v>
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
@@ -5844,8 +5841,8 @@
       <c r="A46">
         <v>44</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>143</v>
+      <c r="B46" t="s">
+        <v>141</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
@@ -5856,8 +5853,8 @@
       <c r="A47">
         <v>45</v>
       </c>
-      <c r="B47" s="12" t="s">
-        <v>144</v>
+      <c r="B47" t="s">
+        <v>142</v>
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
@@ -5868,8 +5865,8 @@
       <c r="A48">
         <v>46</v>
       </c>
-      <c r="B48" s="12" t="s">
-        <v>145</v>
+      <c r="B48" t="s">
+        <v>143</v>
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
@@ -5880,8 +5877,8 @@
       <c r="A49">
         <v>47</v>
       </c>
-      <c r="B49" s="12" t="s">
-        <v>146</v>
+      <c r="B49" t="s">
+        <v>144</v>
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
@@ -5892,8 +5889,8 @@
       <c r="A50">
         <v>48</v>
       </c>
-      <c r="B50" s="12" t="s">
-        <v>147</v>
+      <c r="B50" t="s">
+        <v>145</v>
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
@@ -5904,8 +5901,8 @@
       <c r="A51">
         <v>49</v>
       </c>
-      <c r="B51" s="12" t="s">
-        <v>148</v>
+      <c r="B51" t="s">
+        <v>146</v>
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
@@ -5916,8 +5913,8 @@
       <c r="A52">
         <v>50</v>
       </c>
-      <c r="B52" s="12" t="s">
-        <v>149</v>
+      <c r="B52" t="s">
+        <v>147</v>
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
@@ -5928,8 +5925,8 @@
       <c r="A53">
         <v>51</v>
       </c>
-      <c r="B53" s="12" t="s">
-        <v>150</v>
+      <c r="B53" t="s">
+        <v>148</v>
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
@@ -5940,8 +5937,8 @@
       <c r="A54">
         <v>52</v>
       </c>
-      <c r="B54" s="12" t="s">
-        <v>151</v>
+      <c r="B54" t="s">
+        <v>149</v>
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
@@ -5952,8 +5949,8 @@
       <c r="A55">
         <v>53</v>
       </c>
-      <c r="B55" s="12" t="s">
-        <v>152</v>
+      <c r="B55" t="s">
+        <v>150</v>
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
@@ -5964,8 +5961,8 @@
       <c r="A56">
         <v>54</v>
       </c>
-      <c r="B56" s="12" t="s">
-        <v>153</v>
+      <c r="B56" t="s">
+        <v>151</v>
       </c>
       <c r="C56">
         <f t="shared" si="0"/>
@@ -5976,8 +5973,8 @@
       <c r="A57">
         <v>55</v>
       </c>
-      <c r="B57" s="12" t="s">
-        <v>154</v>
+      <c r="B57" t="s">
+        <v>152</v>
       </c>
       <c r="C57">
         <f t="shared" si="0"/>
@@ -5988,8 +5985,8 @@
       <c r="A58">
         <v>56</v>
       </c>
-      <c r="B58" s="12" t="s">
-        <v>155</v>
+      <c r="B58" t="s">
+        <v>153</v>
       </c>
       <c r="C58">
         <f t="shared" si="0"/>
@@ -6000,8 +5997,8 @@
       <c r="A59">
         <v>57</v>
       </c>
-      <c r="B59" s="12" t="s">
-        <v>156</v>
+      <c r="B59" t="s">
+        <v>154</v>
       </c>
       <c r="C59">
         <f t="shared" si="0"/>
@@ -6012,8 +6009,8 @@
       <c r="A60">
         <v>58</v>
       </c>
-      <c r="B60" s="12" t="s">
-        <v>157</v>
+      <c r="B60" t="s">
+        <v>155</v>
       </c>
       <c r="C60">
         <f t="shared" si="0"/>
@@ -6024,8 +6021,8 @@
       <c r="A61">
         <v>59</v>
       </c>
-      <c r="B61" s="12" t="s">
-        <v>158</v>
+      <c r="B61" t="s">
+        <v>156</v>
       </c>
       <c r="C61">
         <f t="shared" si="0"/>
@@ -6036,8 +6033,8 @@
       <c r="A62">
         <v>60</v>
       </c>
-      <c r="B62" s="12" t="s">
-        <v>159</v>
+      <c r="B62" t="s">
+        <v>157</v>
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
@@ -6048,8 +6045,8 @@
       <c r="A63">
         <v>61</v>
       </c>
-      <c r="B63" s="12" t="s">
-        <v>160</v>
+      <c r="B63" t="s">
+        <v>158</v>
       </c>
       <c r="C63">
         <f t="shared" si="0"/>
@@ -6060,8 +6057,8 @@
       <c r="A64">
         <v>62</v>
       </c>
-      <c r="B64" s="12" t="s">
-        <v>161</v>
+      <c r="B64" t="s">
+        <v>159</v>
       </c>
       <c r="C64">
         <f t="shared" si="0"/>
@@ -6072,8 +6069,8 @@
       <c r="A65">
         <v>63</v>
       </c>
-      <c r="B65" s="12" t="s">
-        <v>162</v>
+      <c r="B65" t="s">
+        <v>160</v>
       </c>
       <c r="C65">
         <f t="shared" si="0"/>
@@ -6084,8 +6081,8 @@
       <c r="A66">
         <v>64</v>
       </c>
-      <c r="B66" s="12" t="s">
-        <v>163</v>
+      <c r="B66" t="s">
+        <v>161</v>
       </c>
       <c r="C66">
         <f t="shared" ref="C66:C129" si="1">VALUE(MID(B66, FIND("(", B66) + 1, FIND(")", B66) - FIND("(", B66) - 1))</f>
@@ -6096,8 +6093,8 @@
       <c r="A67">
         <v>65</v>
       </c>
-      <c r="B67" s="12" t="s">
-        <v>164</v>
+      <c r="B67" t="s">
+        <v>162</v>
       </c>
       <c r="C67">
         <f t="shared" si="1"/>
@@ -6108,8 +6105,8 @@
       <c r="A68">
         <v>66</v>
       </c>
-      <c r="B68" s="12" t="s">
-        <v>165</v>
+      <c r="B68" t="s">
+        <v>163</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
@@ -6120,8 +6117,8 @@
       <c r="A69">
         <v>67</v>
       </c>
-      <c r="B69" s="12" t="s">
-        <v>166</v>
+      <c r="B69" t="s">
+        <v>164</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
@@ -6132,8 +6129,8 @@
       <c r="A70">
         <v>68</v>
       </c>
-      <c r="B70" s="12" t="s">
-        <v>167</v>
+      <c r="B70" t="s">
+        <v>165</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
@@ -6144,8 +6141,8 @@
       <c r="A71">
         <v>69</v>
       </c>
-      <c r="B71" s="12" t="s">
-        <v>168</v>
+      <c r="B71" t="s">
+        <v>166</v>
       </c>
       <c r="C71">
         <f t="shared" si="1"/>
@@ -6156,8 +6153,8 @@
       <c r="A72">
         <v>70</v>
       </c>
-      <c r="B72" s="12" t="s">
-        <v>169</v>
+      <c r="B72" t="s">
+        <v>167</v>
       </c>
       <c r="C72">
         <f t="shared" si="1"/>
@@ -6168,8 +6165,8 @@
       <c r="A73">
         <v>71</v>
       </c>
-      <c r="B73" s="12" t="s">
-        <v>170</v>
+      <c r="B73" t="s">
+        <v>168</v>
       </c>
       <c r="C73">
         <f t="shared" si="1"/>
@@ -6180,8 +6177,8 @@
       <c r="A74">
         <v>72</v>
       </c>
-      <c r="B74" s="12" t="s">
-        <v>171</v>
+      <c r="B74" t="s">
+        <v>169</v>
       </c>
       <c r="C74">
         <f t="shared" si="1"/>
@@ -6192,8 +6189,8 @@
       <c r="A75">
         <v>73</v>
       </c>
-      <c r="B75" s="12" t="s">
-        <v>172</v>
+      <c r="B75" t="s">
+        <v>170</v>
       </c>
       <c r="C75">
         <f t="shared" si="1"/>
@@ -6204,8 +6201,8 @@
       <c r="A76">
         <v>74</v>
       </c>
-      <c r="B76" s="12" t="s">
-        <v>173</v>
+      <c r="B76" t="s">
+        <v>171</v>
       </c>
       <c r="C76">
         <f t="shared" si="1"/>
@@ -6216,8 +6213,8 @@
       <c r="A77">
         <v>75</v>
       </c>
-      <c r="B77" s="12" t="s">
-        <v>174</v>
+      <c r="B77" t="s">
+        <v>172</v>
       </c>
       <c r="C77">
         <f t="shared" si="1"/>
@@ -6228,8 +6225,8 @@
       <c r="A78">
         <v>76</v>
       </c>
-      <c r="B78" s="12" t="s">
-        <v>175</v>
+      <c r="B78" t="s">
+        <v>173</v>
       </c>
       <c r="C78">
         <f t="shared" si="1"/>
@@ -6240,8 +6237,8 @@
       <c r="A79">
         <v>77</v>
       </c>
-      <c r="B79" s="12" t="s">
-        <v>176</v>
+      <c r="B79" t="s">
+        <v>174</v>
       </c>
       <c r="C79">
         <f t="shared" si="1"/>
@@ -6252,8 +6249,8 @@
       <c r="A80">
         <v>78</v>
       </c>
-      <c r="B80" s="12" t="s">
-        <v>177</v>
+      <c r="B80" t="s">
+        <v>175</v>
       </c>
       <c r="C80">
         <f t="shared" si="1"/>
@@ -6264,8 +6261,8 @@
       <c r="A81">
         <v>79</v>
       </c>
-      <c r="B81" s="12" t="s">
-        <v>178</v>
+      <c r="B81" t="s">
+        <v>176</v>
       </c>
       <c r="C81">
         <f t="shared" si="1"/>
@@ -6276,8 +6273,8 @@
       <c r="A82">
         <v>80</v>
       </c>
-      <c r="B82" s="12" t="s">
-        <v>179</v>
+      <c r="B82" t="s">
+        <v>177</v>
       </c>
       <c r="C82">
         <f t="shared" si="1"/>
@@ -6288,8 +6285,8 @@
       <c r="A83">
         <v>81</v>
       </c>
-      <c r="B83" s="12" t="s">
-        <v>180</v>
+      <c r="B83" t="s">
+        <v>178</v>
       </c>
       <c r="C83">
         <f t="shared" si="1"/>
@@ -6300,8 +6297,8 @@
       <c r="A84">
         <v>82</v>
       </c>
-      <c r="B84" s="12" t="s">
-        <v>181</v>
+      <c r="B84" t="s">
+        <v>179</v>
       </c>
       <c r="C84">
         <f t="shared" si="1"/>
@@ -6312,8 +6309,8 @@
       <c r="A85">
         <v>83</v>
       </c>
-      <c r="B85" s="12" t="s">
-        <v>182</v>
+      <c r="B85" t="s">
+        <v>180</v>
       </c>
       <c r="C85">
         <f t="shared" si="1"/>
@@ -6324,8 +6321,8 @@
       <c r="A86">
         <v>84</v>
       </c>
-      <c r="B86" s="12" t="s">
-        <v>183</v>
+      <c r="B86" t="s">
+        <v>181</v>
       </c>
       <c r="C86">
         <f t="shared" si="1"/>
@@ -6336,8 +6333,8 @@
       <c r="A87">
         <v>85</v>
       </c>
-      <c r="B87" s="12" t="s">
-        <v>184</v>
+      <c r="B87" t="s">
+        <v>182</v>
       </c>
       <c r="C87">
         <f t="shared" si="1"/>
@@ -6348,8 +6345,8 @@
       <c r="A88">
         <v>86</v>
       </c>
-      <c r="B88" s="12" t="s">
-        <v>185</v>
+      <c r="B88" t="s">
+        <v>183</v>
       </c>
       <c r="C88">
         <f t="shared" si="1"/>
@@ -6360,8 +6357,8 @@
       <c r="A89">
         <v>87</v>
       </c>
-      <c r="B89" s="12" t="s">
-        <v>186</v>
+      <c r="B89" t="s">
+        <v>184</v>
       </c>
       <c r="C89">
         <f t="shared" si="1"/>
@@ -6372,8 +6369,8 @@
       <c r="A90">
         <v>88</v>
       </c>
-      <c r="B90" s="12" t="s">
-        <v>187</v>
+      <c r="B90" t="s">
+        <v>185</v>
       </c>
       <c r="C90">
         <f t="shared" si="1"/>
@@ -6384,8 +6381,8 @@
       <c r="A91">
         <v>89</v>
       </c>
-      <c r="B91" s="12" t="s">
-        <v>188</v>
+      <c r="B91" t="s">
+        <v>186</v>
       </c>
       <c r="C91">
         <f t="shared" si="1"/>
@@ -6396,8 +6393,8 @@
       <c r="A92">
         <v>90</v>
       </c>
-      <c r="B92" s="12" t="s">
-        <v>189</v>
+      <c r="B92" t="s">
+        <v>187</v>
       </c>
       <c r="C92">
         <f t="shared" si="1"/>
@@ -6408,8 +6405,8 @@
       <c r="A93">
         <v>91</v>
       </c>
-      <c r="B93" s="12" t="s">
-        <v>190</v>
+      <c r="B93" t="s">
+        <v>188</v>
       </c>
       <c r="C93">
         <f t="shared" si="1"/>
@@ -6420,8 +6417,8 @@
       <c r="A94">
         <v>92</v>
       </c>
-      <c r="B94" s="12" t="s">
-        <v>191</v>
+      <c r="B94" t="s">
+        <v>189</v>
       </c>
       <c r="C94">
         <f t="shared" si="1"/>
@@ -6432,8 +6429,8 @@
       <c r="A95">
         <v>93</v>
       </c>
-      <c r="B95" s="12" t="s">
-        <v>192</v>
+      <c r="B95" t="s">
+        <v>190</v>
       </c>
       <c r="C95">
         <f t="shared" si="1"/>
@@ -6444,8 +6441,8 @@
       <c r="A96">
         <v>94</v>
       </c>
-      <c r="B96" s="12" t="s">
-        <v>193</v>
+      <c r="B96" t="s">
+        <v>191</v>
       </c>
       <c r="C96">
         <f t="shared" si="1"/>
@@ -6456,8 +6453,8 @@
       <c r="A97">
         <v>95</v>
       </c>
-      <c r="B97" s="12" t="s">
-        <v>194</v>
+      <c r="B97" t="s">
+        <v>192</v>
       </c>
       <c r="C97">
         <f t="shared" si="1"/>
@@ -6468,8 +6465,8 @@
       <c r="A98">
         <v>96</v>
       </c>
-      <c r="B98" s="12" t="s">
-        <v>195</v>
+      <c r="B98" t="s">
+        <v>193</v>
       </c>
       <c r="C98">
         <f t="shared" si="1"/>
@@ -6480,8 +6477,8 @@
       <c r="A99">
         <v>97</v>
       </c>
-      <c r="B99" s="12" t="s">
-        <v>196</v>
+      <c r="B99" t="s">
+        <v>194</v>
       </c>
       <c r="C99">
         <f t="shared" si="1"/>
@@ -6492,8 +6489,8 @@
       <c r="A100">
         <v>98</v>
       </c>
-      <c r="B100" s="12" t="s">
-        <v>197</v>
+      <c r="B100" t="s">
+        <v>195</v>
       </c>
       <c r="C100">
         <f t="shared" si="1"/>
@@ -6504,8 +6501,8 @@
       <c r="A101">
         <v>99</v>
       </c>
-      <c r="B101" s="12" t="s">
-        <v>198</v>
+      <c r="B101" t="s">
+        <v>196</v>
       </c>
       <c r="C101">
         <f t="shared" si="1"/>
@@ -6516,8 +6513,8 @@
       <c r="A102">
         <v>100</v>
       </c>
-      <c r="B102" s="12" t="s">
-        <v>199</v>
+      <c r="B102" t="s">
+        <v>197</v>
       </c>
       <c r="C102">
         <f t="shared" si="1"/>
@@ -6528,8 +6525,8 @@
       <c r="A103">
         <v>101</v>
       </c>
-      <c r="B103" s="12" t="s">
-        <v>200</v>
+      <c r="B103" t="s">
+        <v>198</v>
       </c>
       <c r="C103">
         <f t="shared" si="1"/>
@@ -6540,8 +6537,8 @@
       <c r="A104">
         <v>102</v>
       </c>
-      <c r="B104" s="12" t="s">
-        <v>201</v>
+      <c r="B104" t="s">
+        <v>199</v>
       </c>
       <c r="C104">
         <f t="shared" si="1"/>
@@ -6552,8 +6549,8 @@
       <c r="A105">
         <v>103</v>
       </c>
-      <c r="B105" s="12" t="s">
-        <v>202</v>
+      <c r="B105" t="s">
+        <v>200</v>
       </c>
       <c r="C105">
         <f t="shared" si="1"/>
@@ -6564,8 +6561,8 @@
       <c r="A106">
         <v>104</v>
       </c>
-      <c r="B106" s="12" t="s">
-        <v>203</v>
+      <c r="B106" t="s">
+        <v>201</v>
       </c>
       <c r="C106">
         <f t="shared" si="1"/>
@@ -6576,8 +6573,8 @@
       <c r="A107">
         <v>105</v>
       </c>
-      <c r="B107" s="12" t="s">
-        <v>204</v>
+      <c r="B107" t="s">
+        <v>202</v>
       </c>
       <c r="C107">
         <f t="shared" si="1"/>
@@ -6588,8 +6585,8 @@
       <c r="A108">
         <v>106</v>
       </c>
-      <c r="B108" s="12" t="s">
-        <v>205</v>
+      <c r="B108" t="s">
+        <v>203</v>
       </c>
       <c r="C108">
         <f t="shared" si="1"/>
@@ -6600,8 +6597,8 @@
       <c r="A109">
         <v>107</v>
       </c>
-      <c r="B109" s="12" t="s">
-        <v>206</v>
+      <c r="B109" t="s">
+        <v>204</v>
       </c>
       <c r="C109">
         <f t="shared" si="1"/>
@@ -6612,8 +6609,8 @@
       <c r="A110">
         <v>108</v>
       </c>
-      <c r="B110" s="12" t="s">
-        <v>207</v>
+      <c r="B110" t="s">
+        <v>205</v>
       </c>
       <c r="C110">
         <f t="shared" si="1"/>
@@ -6624,8 +6621,8 @@
       <c r="A111">
         <v>109</v>
       </c>
-      <c r="B111" s="12" t="s">
-        <v>208</v>
+      <c r="B111" t="s">
+        <v>206</v>
       </c>
       <c r="C111">
         <f t="shared" si="1"/>
@@ -6636,8 +6633,8 @@
       <c r="A112">
         <v>110</v>
       </c>
-      <c r="B112" s="12" t="s">
-        <v>209</v>
+      <c r="B112" t="s">
+        <v>207</v>
       </c>
       <c r="C112">
         <f t="shared" si="1"/>
@@ -6648,8 +6645,8 @@
       <c r="A113">
         <v>111</v>
       </c>
-      <c r="B113" s="12" t="s">
-        <v>210</v>
+      <c r="B113" t="s">
+        <v>208</v>
       </c>
       <c r="C113">
         <f t="shared" si="1"/>
@@ -6660,8 +6657,8 @@
       <c r="A114">
         <v>112</v>
       </c>
-      <c r="B114" s="12" t="s">
-        <v>211</v>
+      <c r="B114" t="s">
+        <v>209</v>
       </c>
       <c r="C114">
         <f t="shared" si="1"/>
@@ -6672,8 +6669,8 @@
       <c r="A115">
         <v>113</v>
       </c>
-      <c r="B115" s="12" t="s">
-        <v>212</v>
+      <c r="B115" t="s">
+        <v>210</v>
       </c>
       <c r="C115">
         <f t="shared" si="1"/>
@@ -6684,8 +6681,8 @@
       <c r="A116">
         <v>114</v>
       </c>
-      <c r="B116" s="12" t="s">
-        <v>213</v>
+      <c r="B116" t="s">
+        <v>211</v>
       </c>
       <c r="C116">
         <f t="shared" si="1"/>
@@ -6696,8 +6693,8 @@
       <c r="A117">
         <v>115</v>
       </c>
-      <c r="B117" s="12" t="s">
-        <v>214</v>
+      <c r="B117" t="s">
+        <v>212</v>
       </c>
       <c r="C117">
         <f t="shared" si="1"/>
@@ -6708,8 +6705,8 @@
       <c r="A118">
         <v>116</v>
       </c>
-      <c r="B118" s="12" t="s">
-        <v>215</v>
+      <c r="B118" t="s">
+        <v>213</v>
       </c>
       <c r="C118">
         <f t="shared" si="1"/>
@@ -6720,8 +6717,8 @@
       <c r="A119">
         <v>117</v>
       </c>
-      <c r="B119" s="12" t="s">
-        <v>216</v>
+      <c r="B119" t="s">
+        <v>214</v>
       </c>
       <c r="C119">
         <f t="shared" si="1"/>
@@ -6732,8 +6729,8 @@
       <c r="A120">
         <v>118</v>
       </c>
-      <c r="B120" s="12" t="s">
-        <v>217</v>
+      <c r="B120" t="s">
+        <v>215</v>
       </c>
       <c r="C120">
         <f t="shared" si="1"/>
@@ -6744,8 +6741,8 @@
       <c r="A121">
         <v>119</v>
       </c>
-      <c r="B121" s="12" t="s">
-        <v>218</v>
+      <c r="B121" t="s">
+        <v>216</v>
       </c>
       <c r="C121">
         <f t="shared" si="1"/>
@@ -6756,8 +6753,8 @@
       <c r="A122">
         <v>120</v>
       </c>
-      <c r="B122" s="12" t="s">
-        <v>219</v>
+      <c r="B122" t="s">
+        <v>217</v>
       </c>
       <c r="C122">
         <f t="shared" si="1"/>
@@ -6768,8 +6765,8 @@
       <c r="A123">
         <v>121</v>
       </c>
-      <c r="B123" s="12" t="s">
-        <v>220</v>
+      <c r="B123" t="s">
+        <v>218</v>
       </c>
       <c r="C123">
         <f t="shared" si="1"/>
@@ -6780,8 +6777,8 @@
       <c r="A124">
         <v>122</v>
       </c>
-      <c r="B124" s="12" t="s">
-        <v>221</v>
+      <c r="B124" t="s">
+        <v>219</v>
       </c>
       <c r="C124">
         <f t="shared" si="1"/>
@@ -6792,8 +6789,8 @@
       <c r="A125">
         <v>123</v>
       </c>
-      <c r="B125" s="12" t="s">
-        <v>222</v>
+      <c r="B125" t="s">
+        <v>220</v>
       </c>
       <c r="C125">
         <f t="shared" si="1"/>
@@ -6804,8 +6801,8 @@
       <c r="A126">
         <v>124</v>
       </c>
-      <c r="B126" s="12" t="s">
-        <v>223</v>
+      <c r="B126" t="s">
+        <v>221</v>
       </c>
       <c r="C126">
         <f t="shared" si="1"/>
@@ -6816,8 +6813,8 @@
       <c r="A127">
         <v>125</v>
       </c>
-      <c r="B127" s="12" t="s">
-        <v>224</v>
+      <c r="B127" t="s">
+        <v>222</v>
       </c>
       <c r="C127">
         <f t="shared" si="1"/>
@@ -6828,8 +6825,8 @@
       <c r="A128">
         <v>126</v>
       </c>
-      <c r="B128" s="12" t="s">
-        <v>225</v>
+      <c r="B128" t="s">
+        <v>223</v>
       </c>
       <c r="C128">
         <f t="shared" si="1"/>
@@ -6840,8 +6837,8 @@
       <c r="A129">
         <v>127</v>
       </c>
-      <c r="B129" s="12" t="s">
-        <v>226</v>
+      <c r="B129" t="s">
+        <v>224</v>
       </c>
       <c r="C129">
         <f t="shared" si="1"/>
@@ -6852,8 +6849,8 @@
       <c r="A130">
         <v>128</v>
       </c>
-      <c r="B130" s="12" t="s">
-        <v>227</v>
+      <c r="B130" t="s">
+        <v>225</v>
       </c>
       <c r="C130">
         <f t="shared" ref="C130:C193" si="2">VALUE(MID(B130, FIND("(", B130) + 1, FIND(")", B130) - FIND("(", B130) - 1))</f>
@@ -6864,8 +6861,8 @@
       <c r="A131">
         <v>129</v>
       </c>
-      <c r="B131" s="12" t="s">
-        <v>228</v>
+      <c r="B131" t="s">
+        <v>226</v>
       </c>
       <c r="C131">
         <f t="shared" si="2"/>
@@ -6876,8 +6873,8 @@
       <c r="A132">
         <v>130</v>
       </c>
-      <c r="B132" s="12" t="s">
-        <v>229</v>
+      <c r="B132" t="s">
+        <v>227</v>
       </c>
       <c r="C132">
         <f t="shared" si="2"/>
@@ -6888,8 +6885,8 @@
       <c r="A133">
         <v>131</v>
       </c>
-      <c r="B133" s="12" t="s">
-        <v>230</v>
+      <c r="B133" t="s">
+        <v>228</v>
       </c>
       <c r="C133">
         <f t="shared" si="2"/>
@@ -6900,8 +6897,8 @@
       <c r="A134">
         <v>132</v>
       </c>
-      <c r="B134" s="12" t="s">
-        <v>231</v>
+      <c r="B134" t="s">
+        <v>229</v>
       </c>
       <c r="C134">
         <f t="shared" si="2"/>
@@ -6912,8 +6909,8 @@
       <c r="A135">
         <v>133</v>
       </c>
-      <c r="B135" s="12" t="s">
-        <v>232</v>
+      <c r="B135" t="s">
+        <v>230</v>
       </c>
       <c r="C135">
         <f t="shared" si="2"/>
@@ -6924,8 +6921,8 @@
       <c r="A136">
         <v>134</v>
       </c>
-      <c r="B136" s="12" t="s">
-        <v>233</v>
+      <c r="B136" t="s">
+        <v>231</v>
       </c>
       <c r="C136">
         <f t="shared" si="2"/>
@@ -6936,8 +6933,8 @@
       <c r="A137">
         <v>135</v>
       </c>
-      <c r="B137" s="12" t="s">
-        <v>234</v>
+      <c r="B137" t="s">
+        <v>232</v>
       </c>
       <c r="C137">
         <f t="shared" si="2"/>
@@ -6948,8 +6945,8 @@
       <c r="A138">
         <v>136</v>
       </c>
-      <c r="B138" s="12" t="s">
-        <v>235</v>
+      <c r="B138" t="s">
+        <v>233</v>
       </c>
       <c r="C138">
         <f t="shared" si="2"/>
@@ -6960,8 +6957,8 @@
       <c r="A139">
         <v>137</v>
       </c>
-      <c r="B139" s="12" t="s">
-        <v>236</v>
+      <c r="B139" t="s">
+        <v>234</v>
       </c>
       <c r="C139">
         <f t="shared" si="2"/>
@@ -6972,8 +6969,8 @@
       <c r="A140">
         <v>138</v>
       </c>
-      <c r="B140" s="12" t="s">
-        <v>237</v>
+      <c r="B140" t="s">
+        <v>235</v>
       </c>
       <c r="C140">
         <f t="shared" si="2"/>
@@ -6984,8 +6981,8 @@
       <c r="A141">
         <v>139</v>
       </c>
-      <c r="B141" s="12" t="s">
-        <v>238</v>
+      <c r="B141" t="s">
+        <v>236</v>
       </c>
       <c r="C141">
         <f t="shared" si="2"/>
@@ -6996,8 +6993,8 @@
       <c r="A142">
         <v>140</v>
       </c>
-      <c r="B142" s="12" t="s">
-        <v>239</v>
+      <c r="B142" t="s">
+        <v>237</v>
       </c>
       <c r="C142">
         <f t="shared" si="2"/>
@@ -7008,8 +7005,8 @@
       <c r="A143">
         <v>141</v>
       </c>
-      <c r="B143" s="12" t="s">
-        <v>240</v>
+      <c r="B143" t="s">
+        <v>238</v>
       </c>
       <c r="C143">
         <f t="shared" si="2"/>
@@ -7020,8 +7017,8 @@
       <c r="A144">
         <v>142</v>
       </c>
-      <c r="B144" s="12" t="s">
-        <v>241</v>
+      <c r="B144" t="s">
+        <v>239</v>
       </c>
       <c r="C144">
         <f t="shared" si="2"/>
@@ -7032,8 +7029,8 @@
       <c r="A145">
         <v>143</v>
       </c>
-      <c r="B145" s="12" t="s">
-        <v>242</v>
+      <c r="B145" t="s">
+        <v>240</v>
       </c>
       <c r="C145">
         <f t="shared" si="2"/>
@@ -7044,8 +7041,8 @@
       <c r="A146">
         <v>144</v>
       </c>
-      <c r="B146" s="12" t="s">
-        <v>243</v>
+      <c r="B146" t="s">
+        <v>241</v>
       </c>
       <c r="C146">
         <f t="shared" si="2"/>
@@ -7056,8 +7053,8 @@
       <c r="A147">
         <v>145</v>
       </c>
-      <c r="B147" s="12" t="s">
-        <v>244</v>
+      <c r="B147" t="s">
+        <v>242</v>
       </c>
       <c r="C147">
         <f t="shared" si="2"/>
@@ -7068,8 +7065,8 @@
       <c r="A148">
         <v>146</v>
       </c>
-      <c r="B148" s="12" t="s">
-        <v>245</v>
+      <c r="B148" t="s">
+        <v>243</v>
       </c>
       <c r="C148">
         <f t="shared" si="2"/>
@@ -7080,8 +7077,8 @@
       <c r="A149">
         <v>147</v>
       </c>
-      <c r="B149" s="12" t="s">
-        <v>246</v>
+      <c r="B149" t="s">
+        <v>244</v>
       </c>
       <c r="C149">
         <f t="shared" si="2"/>
@@ -7092,8 +7089,8 @@
       <c r="A150">
         <v>148</v>
       </c>
-      <c r="B150" s="12" t="s">
-        <v>247</v>
+      <c r="B150" t="s">
+        <v>245</v>
       </c>
       <c r="C150">
         <f t="shared" si="2"/>
@@ -7104,8 +7101,8 @@
       <c r="A151">
         <v>149</v>
       </c>
-      <c r="B151" s="12" t="s">
-        <v>248</v>
+      <c r="B151" t="s">
+        <v>246</v>
       </c>
       <c r="C151">
         <f t="shared" si="2"/>
@@ -7116,8 +7113,8 @@
       <c r="A152">
         <v>150</v>
       </c>
-      <c r="B152" s="12" t="s">
-        <v>249</v>
+      <c r="B152" t="s">
+        <v>247</v>
       </c>
       <c r="C152">
         <f t="shared" si="2"/>
@@ -7128,8 +7125,8 @@
       <c r="A153">
         <v>151</v>
       </c>
-      <c r="B153" s="12" t="s">
-        <v>250</v>
+      <c r="B153" t="s">
+        <v>248</v>
       </c>
       <c r="C153">
         <f t="shared" si="2"/>
@@ -7140,8 +7137,8 @@
       <c r="A154">
         <v>152</v>
       </c>
-      <c r="B154" s="12" t="s">
-        <v>251</v>
+      <c r="B154" t="s">
+        <v>249</v>
       </c>
       <c r="C154">
         <f t="shared" si="2"/>
@@ -7152,8 +7149,8 @@
       <c r="A155">
         <v>153</v>
       </c>
-      <c r="B155" s="12" t="s">
-        <v>252</v>
+      <c r="B155" t="s">
+        <v>250</v>
       </c>
       <c r="C155">
         <f t="shared" si="2"/>
@@ -7164,8 +7161,8 @@
       <c r="A156">
         <v>154</v>
       </c>
-      <c r="B156" s="12" t="s">
-        <v>253</v>
+      <c r="B156" t="s">
+        <v>251</v>
       </c>
       <c r="C156">
         <f t="shared" si="2"/>
@@ -7176,8 +7173,8 @@
       <c r="A157">
         <v>155</v>
       </c>
-      <c r="B157" s="12" t="s">
-        <v>254</v>
+      <c r="B157" t="s">
+        <v>252</v>
       </c>
       <c r="C157">
         <f t="shared" si="2"/>
@@ -7188,8 +7185,8 @@
       <c r="A158">
         <v>156</v>
       </c>
-      <c r="B158" s="12" t="s">
-        <v>255</v>
+      <c r="B158" t="s">
+        <v>253</v>
       </c>
       <c r="C158">
         <f t="shared" si="2"/>
@@ -7200,8 +7197,8 @@
       <c r="A159">
         <v>157</v>
       </c>
-      <c r="B159" s="12" t="s">
-        <v>256</v>
+      <c r="B159" t="s">
+        <v>254</v>
       </c>
       <c r="C159">
         <f t="shared" si="2"/>
@@ -7212,8 +7209,8 @@
       <c r="A160">
         <v>158</v>
       </c>
-      <c r="B160" s="12" t="s">
-        <v>257</v>
+      <c r="B160" t="s">
+        <v>255</v>
       </c>
       <c r="C160">
         <f t="shared" si="2"/>
@@ -7224,8 +7221,8 @@
       <c r="A161">
         <v>159</v>
       </c>
-      <c r="B161" s="12" t="s">
-        <v>258</v>
+      <c r="B161" t="s">
+        <v>256</v>
       </c>
       <c r="C161">
         <f t="shared" si="2"/>
@@ -7236,8 +7233,8 @@
       <c r="A162">
         <v>160</v>
       </c>
-      <c r="B162" s="12" t="s">
-        <v>259</v>
+      <c r="B162" t="s">
+        <v>257</v>
       </c>
       <c r="C162">
         <f t="shared" si="2"/>
@@ -7248,8 +7245,8 @@
       <c r="A163">
         <v>161</v>
       </c>
-      <c r="B163" s="12" t="s">
-        <v>260</v>
+      <c r="B163" t="s">
+        <v>258</v>
       </c>
       <c r="C163">
         <f t="shared" si="2"/>
@@ -7260,8 +7257,8 @@
       <c r="A164">
         <v>162</v>
       </c>
-      <c r="B164" s="12" t="s">
-        <v>261</v>
+      <c r="B164" t="s">
+        <v>259</v>
       </c>
       <c r="C164">
         <f t="shared" si="2"/>
@@ -7272,8 +7269,8 @@
       <c r="A165">
         <v>163</v>
       </c>
-      <c r="B165" s="12" t="s">
-        <v>262</v>
+      <c r="B165" t="s">
+        <v>260</v>
       </c>
       <c r="C165">
         <f t="shared" si="2"/>
@@ -7284,8 +7281,8 @@
       <c r="A166">
         <v>164</v>
       </c>
-      <c r="B166" s="12" t="s">
-        <v>263</v>
+      <c r="B166" t="s">
+        <v>261</v>
       </c>
       <c r="C166">
         <f t="shared" si="2"/>
@@ -7296,8 +7293,8 @@
       <c r="A167">
         <v>165</v>
       </c>
-      <c r="B167" s="12" t="s">
-        <v>264</v>
+      <c r="B167" t="s">
+        <v>262</v>
       </c>
       <c r="C167">
         <f t="shared" si="2"/>
@@ -7308,8 +7305,8 @@
       <c r="A168">
         <v>166</v>
       </c>
-      <c r="B168" s="12" t="s">
-        <v>265</v>
+      <c r="B168" t="s">
+        <v>263</v>
       </c>
       <c r="C168">
         <f t="shared" si="2"/>
@@ -7320,8 +7317,8 @@
       <c r="A169">
         <v>167</v>
       </c>
-      <c r="B169" s="12" t="s">
-        <v>266</v>
+      <c r="B169" t="s">
+        <v>264</v>
       </c>
       <c r="C169">
         <f t="shared" si="2"/>
@@ -7332,8 +7329,8 @@
       <c r="A170">
         <v>168</v>
       </c>
-      <c r="B170" s="12" t="s">
-        <v>267</v>
+      <c r="B170" t="s">
+        <v>265</v>
       </c>
       <c r="C170">
         <f t="shared" si="2"/>
@@ -7344,8 +7341,8 @@
       <c r="A171">
         <v>169</v>
       </c>
-      <c r="B171" s="12" t="s">
-        <v>268</v>
+      <c r="B171" t="s">
+        <v>266</v>
       </c>
       <c r="C171">
         <f t="shared" si="2"/>
@@ -7356,8 +7353,8 @@
       <c r="A172">
         <v>170</v>
       </c>
-      <c r="B172" s="12" t="s">
-        <v>269</v>
+      <c r="B172" t="s">
+        <v>267</v>
       </c>
       <c r="C172">
         <f t="shared" si="2"/>
@@ -7368,8 +7365,8 @@
       <c r="A173">
         <v>171</v>
       </c>
-      <c r="B173" s="12" t="s">
-        <v>270</v>
+      <c r="B173" t="s">
+        <v>268</v>
       </c>
       <c r="C173">
         <f t="shared" si="2"/>
@@ -7380,8 +7377,8 @@
       <c r="A174">
         <v>172</v>
       </c>
-      <c r="B174" s="12" t="s">
-        <v>271</v>
+      <c r="B174" t="s">
+        <v>269</v>
       </c>
       <c r="C174">
         <f t="shared" si="2"/>
@@ -7392,8 +7389,8 @@
       <c r="A175">
         <v>173</v>
       </c>
-      <c r="B175" s="12" t="s">
-        <v>272</v>
+      <c r="B175" t="s">
+        <v>270</v>
       </c>
       <c r="C175">
         <f t="shared" si="2"/>
@@ -7404,8 +7401,8 @@
       <c r="A176">
         <v>174</v>
       </c>
-      <c r="B176" s="12" t="s">
-        <v>273</v>
+      <c r="B176" t="s">
+        <v>271</v>
       </c>
       <c r="C176">
         <f t="shared" si="2"/>
@@ -7416,8 +7413,8 @@
       <c r="A177">
         <v>175</v>
       </c>
-      <c r="B177" s="12" t="s">
-        <v>274</v>
+      <c r="B177" t="s">
+        <v>272</v>
       </c>
       <c r="C177">
         <f t="shared" si="2"/>
@@ -7428,8 +7425,8 @@
       <c r="A178">
         <v>176</v>
       </c>
-      <c r="B178" s="12" t="s">
-        <v>275</v>
+      <c r="B178" t="s">
+        <v>273</v>
       </c>
       <c r="C178">
         <f t="shared" si="2"/>
@@ -7440,8 +7437,8 @@
       <c r="A179">
         <v>177</v>
       </c>
-      <c r="B179" s="12" t="s">
-        <v>276</v>
+      <c r="B179" t="s">
+        <v>274</v>
       </c>
       <c r="C179">
         <f t="shared" si="2"/>
@@ -7452,8 +7449,8 @@
       <c r="A180">
         <v>178</v>
       </c>
-      <c r="B180" s="12" t="s">
-        <v>277</v>
+      <c r="B180" t="s">
+        <v>275</v>
       </c>
       <c r="C180">
         <f t="shared" si="2"/>
@@ -7464,8 +7461,8 @@
       <c r="A181">
         <v>179</v>
       </c>
-      <c r="B181" s="12" t="s">
-        <v>278</v>
+      <c r="B181" t="s">
+        <v>276</v>
       </c>
       <c r="C181">
         <f t="shared" si="2"/>
@@ -7476,8 +7473,8 @@
       <c r="A182">
         <v>180</v>
       </c>
-      <c r="B182" s="12" t="s">
-        <v>279</v>
+      <c r="B182" t="s">
+        <v>277</v>
       </c>
       <c r="C182">
         <f t="shared" si="2"/>
@@ -7488,8 +7485,8 @@
       <c r="A183">
         <v>181</v>
       </c>
-      <c r="B183" s="12" t="s">
-        <v>280</v>
+      <c r="B183" t="s">
+        <v>278</v>
       </c>
       <c r="C183">
         <f t="shared" si="2"/>
@@ -7500,8 +7497,8 @@
       <c r="A184">
         <v>182</v>
       </c>
-      <c r="B184" s="12" t="s">
-        <v>281</v>
+      <c r="B184" t="s">
+        <v>279</v>
       </c>
       <c r="C184">
         <f t="shared" si="2"/>
@@ -7512,8 +7509,8 @@
       <c r="A185">
         <v>183</v>
       </c>
-      <c r="B185" s="12" t="s">
-        <v>214</v>
+      <c r="B185" t="s">
+        <v>212</v>
       </c>
       <c r="C185">
         <f t="shared" si="2"/>
@@ -7524,8 +7521,8 @@
       <c r="A186">
         <v>184</v>
       </c>
-      <c r="B186" s="12" t="s">
-        <v>282</v>
+      <c r="B186" t="s">
+        <v>280</v>
       </c>
       <c r="C186">
         <f t="shared" si="2"/>
@@ -7536,8 +7533,8 @@
       <c r="A187">
         <v>185</v>
       </c>
-      <c r="B187" s="12" t="s">
-        <v>283</v>
+      <c r="B187" t="s">
+        <v>281</v>
       </c>
       <c r="C187">
         <f t="shared" si="2"/>
@@ -7548,8 +7545,8 @@
       <c r="A188">
         <v>186</v>
       </c>
-      <c r="B188" s="12" t="s">
-        <v>284</v>
+      <c r="B188" t="s">
+        <v>282</v>
       </c>
       <c r="C188">
         <f t="shared" si="2"/>
@@ -7560,8 +7557,8 @@
       <c r="A189">
         <v>187</v>
       </c>
-      <c r="B189" s="12" t="s">
-        <v>285</v>
+      <c r="B189" t="s">
+        <v>283</v>
       </c>
       <c r="C189">
         <f t="shared" si="2"/>
@@ -7572,8 +7569,8 @@
       <c r="A190">
         <v>188</v>
       </c>
-      <c r="B190" s="12" t="s">
-        <v>286</v>
+      <c r="B190" t="s">
+        <v>284</v>
       </c>
       <c r="C190">
         <f t="shared" si="2"/>
@@ -7584,8 +7581,8 @@
       <c r="A191">
         <v>189</v>
       </c>
-      <c r="B191" s="12" t="s">
-        <v>287</v>
+      <c r="B191" t="s">
+        <v>285</v>
       </c>
       <c r="C191">
         <f t="shared" si="2"/>
@@ -7596,8 +7593,8 @@
       <c r="A192">
         <v>190</v>
       </c>
-      <c r="B192" s="12" t="s">
-        <v>288</v>
+      <c r="B192" t="s">
+        <v>286</v>
       </c>
       <c r="C192">
         <f t="shared" si="2"/>
@@ -7608,8 +7605,8 @@
       <c r="A193">
         <v>191</v>
       </c>
-      <c r="B193" s="12" t="s">
-        <v>289</v>
+      <c r="B193" t="s">
+        <v>287</v>
       </c>
       <c r="C193">
         <f t="shared" si="2"/>
@@ -7620,8 +7617,8 @@
       <c r="A194">
         <v>192</v>
       </c>
-      <c r="B194" s="12" t="s">
-        <v>290</v>
+      <c r="B194" t="s">
+        <v>288</v>
       </c>
       <c r="C194">
         <f t="shared" ref="C194:C257" si="3">VALUE(MID(B194, FIND("(", B194) + 1, FIND(")", B194) - FIND("(", B194) - 1))</f>
@@ -7632,8 +7629,8 @@
       <c r="A195">
         <v>193</v>
       </c>
-      <c r="B195" s="12" t="s">
-        <v>291</v>
+      <c r="B195" t="s">
+        <v>289</v>
       </c>
       <c r="C195">
         <f t="shared" si="3"/>
@@ -7644,8 +7641,8 @@
       <c r="A196">
         <v>194</v>
       </c>
-      <c r="B196" s="12" t="s">
-        <v>292</v>
+      <c r="B196" t="s">
+        <v>290</v>
       </c>
       <c r="C196">
         <f t="shared" si="3"/>
@@ -7656,8 +7653,8 @@
       <c r="A197">
         <v>195</v>
       </c>
-      <c r="B197" s="12" t="s">
-        <v>293</v>
+      <c r="B197" t="s">
+        <v>291</v>
       </c>
       <c r="C197">
         <f t="shared" si="3"/>
@@ -7668,8 +7665,8 @@
       <c r="A198">
         <v>196</v>
       </c>
-      <c r="B198" s="12" t="s">
-        <v>294</v>
+      <c r="B198" t="s">
+        <v>292</v>
       </c>
       <c r="C198">
         <f t="shared" si="3"/>
@@ -7680,8 +7677,8 @@
       <c r="A199">
         <v>197</v>
       </c>
-      <c r="B199" s="12" t="s">
-        <v>295</v>
+      <c r="B199" t="s">
+        <v>293</v>
       </c>
       <c r="C199">
         <f t="shared" si="3"/>
@@ -7692,8 +7689,8 @@
       <c r="A200">
         <v>198</v>
       </c>
-      <c r="B200" s="12" t="s">
-        <v>296</v>
+      <c r="B200" t="s">
+        <v>294</v>
       </c>
       <c r="C200">
         <f t="shared" si="3"/>
@@ -7704,8 +7701,8 @@
       <c r="A201">
         <v>199</v>
       </c>
-      <c r="B201" s="12" t="s">
-        <v>297</v>
+      <c r="B201" t="s">
+        <v>295</v>
       </c>
       <c r="C201">
         <f t="shared" si="3"/>
@@ -7716,8 +7713,8 @@
       <c r="A202">
         <v>200</v>
       </c>
-      <c r="B202" s="12" t="s">
-        <v>298</v>
+      <c r="B202" t="s">
+        <v>296</v>
       </c>
       <c r="C202">
         <f t="shared" si="3"/>
@@ -7728,8 +7725,8 @@
       <c r="A203">
         <v>201</v>
       </c>
-      <c r="B203" s="12" t="s">
-        <v>299</v>
+      <c r="B203" t="s">
+        <v>297</v>
       </c>
       <c r="C203">
         <f t="shared" si="3"/>
@@ -7740,8 +7737,8 @@
       <c r="A204">
         <v>202</v>
       </c>
-      <c r="B204" s="12" t="s">
-        <v>300</v>
+      <c r="B204" t="s">
+        <v>298</v>
       </c>
       <c r="C204">
         <f t="shared" si="3"/>
@@ -7752,8 +7749,8 @@
       <c r="A205">
         <v>203</v>
       </c>
-      <c r="B205" s="12" t="s">
-        <v>301</v>
+      <c r="B205" t="s">
+        <v>299</v>
       </c>
       <c r="C205">
         <f t="shared" si="3"/>
@@ -7764,8 +7761,8 @@
       <c r="A206">
         <v>204</v>
       </c>
-      <c r="B206" s="12" t="s">
-        <v>302</v>
+      <c r="B206" t="s">
+        <v>300</v>
       </c>
       <c r="C206">
         <f t="shared" si="3"/>
@@ -7776,8 +7773,8 @@
       <c r="A207">
         <v>205</v>
       </c>
-      <c r="B207" s="12" t="s">
-        <v>303</v>
+      <c r="B207" t="s">
+        <v>301</v>
       </c>
       <c r="C207">
         <f t="shared" si="3"/>
@@ -7788,8 +7785,8 @@
       <c r="A208">
         <v>206</v>
       </c>
-      <c r="B208" s="12" t="s">
-        <v>304</v>
+      <c r="B208" t="s">
+        <v>302</v>
       </c>
       <c r="C208">
         <f t="shared" si="3"/>
@@ -7800,8 +7797,8 @@
       <c r="A209">
         <v>207</v>
       </c>
-      <c r="B209" s="12" t="s">
-        <v>305</v>
+      <c r="B209" t="s">
+        <v>303</v>
       </c>
       <c r="C209">
         <f t="shared" si="3"/>
@@ -7812,8 +7809,8 @@
       <c r="A210">
         <v>208</v>
       </c>
-      <c r="B210" s="12" t="s">
-        <v>306</v>
+      <c r="B210" t="s">
+        <v>304</v>
       </c>
       <c r="C210">
         <f t="shared" si="3"/>
@@ -7824,8 +7821,8 @@
       <c r="A211">
         <v>209</v>
       </c>
-      <c r="B211" s="12" t="s">
-        <v>307</v>
+      <c r="B211" t="s">
+        <v>305</v>
       </c>
       <c r="C211">
         <f t="shared" si="3"/>
@@ -7836,8 +7833,8 @@
       <c r="A212">
         <v>210</v>
       </c>
-      <c r="B212" s="12" t="s">
-        <v>308</v>
+      <c r="B212" t="s">
+        <v>306</v>
       </c>
       <c r="C212">
         <f t="shared" si="3"/>
@@ -7848,8 +7845,8 @@
       <c r="A213">
         <v>211</v>
       </c>
-      <c r="B213" s="12" t="s">
-        <v>309</v>
+      <c r="B213" t="s">
+        <v>307</v>
       </c>
       <c r="C213">
         <f t="shared" si="3"/>
@@ -7860,8 +7857,8 @@
       <c r="A214">
         <v>212</v>
       </c>
-      <c r="B214" s="12" t="s">
-        <v>310</v>
+      <c r="B214" t="s">
+        <v>308</v>
       </c>
       <c r="C214">
         <f t="shared" si="3"/>
@@ -7872,8 +7869,8 @@
       <c r="A215">
         <v>213</v>
       </c>
-      <c r="B215" s="12" t="s">
-        <v>311</v>
+      <c r="B215" t="s">
+        <v>309</v>
       </c>
       <c r="C215">
         <f t="shared" si="3"/>
@@ -7884,8 +7881,8 @@
       <c r="A216">
         <v>214</v>
       </c>
-      <c r="B216" s="12" t="s">
-        <v>312</v>
+      <c r="B216" t="s">
+        <v>310</v>
       </c>
       <c r="C216">
         <f t="shared" si="3"/>
@@ -7896,8 +7893,8 @@
       <c r="A217">
         <v>215</v>
       </c>
-      <c r="B217" s="12" t="s">
-        <v>313</v>
+      <c r="B217" t="s">
+        <v>311</v>
       </c>
       <c r="C217">
         <f t="shared" si="3"/>
@@ -7908,8 +7905,8 @@
       <c r="A218">
         <v>216</v>
       </c>
-      <c r="B218" s="12" t="s">
-        <v>314</v>
+      <c r="B218" t="s">
+        <v>312</v>
       </c>
       <c r="C218">
         <f t="shared" si="3"/>
@@ -7920,8 +7917,8 @@
       <c r="A219">
         <v>217</v>
       </c>
-      <c r="B219" s="12" t="s">
-        <v>315</v>
+      <c r="B219" t="s">
+        <v>313</v>
       </c>
       <c r="C219">
         <f t="shared" si="3"/>
@@ -7932,8 +7929,8 @@
       <c r="A220">
         <v>218</v>
       </c>
-      <c r="B220" s="12" t="s">
-        <v>316</v>
+      <c r="B220" t="s">
+        <v>314</v>
       </c>
       <c r="C220">
         <f t="shared" si="3"/>
@@ -7944,8 +7941,8 @@
       <c r="A221">
         <v>219</v>
       </c>
-      <c r="B221" s="12" t="s">
-        <v>317</v>
+      <c r="B221" t="s">
+        <v>315</v>
       </c>
       <c r="C221">
         <f t="shared" si="3"/>
@@ -7956,8 +7953,8 @@
       <c r="A222">
         <v>220</v>
       </c>
-      <c r="B222" s="12" t="s">
-        <v>318</v>
+      <c r="B222" t="s">
+        <v>316</v>
       </c>
       <c r="C222">
         <f t="shared" si="3"/>
@@ -7968,8 +7965,8 @@
       <c r="A223">
         <v>221</v>
       </c>
-      <c r="B223" s="12" t="s">
-        <v>319</v>
+      <c r="B223" t="s">
+        <v>317</v>
       </c>
       <c r="C223">
         <f t="shared" si="3"/>
@@ -7980,8 +7977,8 @@
       <c r="A224">
         <v>222</v>
       </c>
-      <c r="B224" s="12" t="s">
-        <v>320</v>
+      <c r="B224" t="s">
+        <v>318</v>
       </c>
       <c r="C224">
         <f t="shared" si="3"/>
@@ -7992,8 +7989,8 @@
       <c r="A225">
         <v>223</v>
       </c>
-      <c r="B225" s="12" t="s">
-        <v>321</v>
+      <c r="B225" t="s">
+        <v>319</v>
       </c>
       <c r="C225">
         <f t="shared" si="3"/>
@@ -8004,8 +8001,8 @@
       <c r="A226">
         <v>224</v>
       </c>
-      <c r="B226" s="12" t="s">
-        <v>322</v>
+      <c r="B226" t="s">
+        <v>320</v>
       </c>
       <c r="C226">
         <f t="shared" si="3"/>
@@ -8016,8 +8013,8 @@
       <c r="A227">
         <v>225</v>
       </c>
-      <c r="B227" s="12" t="s">
-        <v>323</v>
+      <c r="B227" t="s">
+        <v>321</v>
       </c>
       <c r="C227">
         <f t="shared" si="3"/>
@@ -8028,8 +8025,8 @@
       <c r="A228">
         <v>226</v>
       </c>
-      <c r="B228" s="12" t="s">
-        <v>324</v>
+      <c r="B228" t="s">
+        <v>322</v>
       </c>
       <c r="C228">
         <f t="shared" si="3"/>
@@ -8040,8 +8037,8 @@
       <c r="A229">
         <v>227</v>
       </c>
-      <c r="B229" s="12" t="s">
-        <v>325</v>
+      <c r="B229" t="s">
+        <v>323</v>
       </c>
       <c r="C229">
         <f t="shared" si="3"/>
@@ -8052,8 +8049,8 @@
       <c r="A230">
         <v>228</v>
       </c>
-      <c r="B230" s="12" t="s">
-        <v>326</v>
+      <c r="B230" t="s">
+        <v>324</v>
       </c>
       <c r="C230">
         <f t="shared" si="3"/>
@@ -8064,8 +8061,8 @@
       <c r="A231">
         <v>229</v>
       </c>
-      <c r="B231" s="12" t="s">
-        <v>327</v>
+      <c r="B231" t="s">
+        <v>325</v>
       </c>
       <c r="C231">
         <f t="shared" si="3"/>
@@ -8076,8 +8073,8 @@
       <c r="A232">
         <v>230</v>
       </c>
-      <c r="B232" s="12" t="s">
-        <v>328</v>
+      <c r="B232" t="s">
+        <v>326</v>
       </c>
       <c r="C232">
         <f t="shared" si="3"/>
@@ -8088,8 +8085,8 @@
       <c r="A233">
         <v>231</v>
       </c>
-      <c r="B233" s="12" t="s">
-        <v>329</v>
+      <c r="B233" t="s">
+        <v>327</v>
       </c>
       <c r="C233">
         <f t="shared" si="3"/>
@@ -8100,8 +8097,8 @@
       <c r="A234">
         <v>232</v>
       </c>
-      <c r="B234" s="12" t="s">
-        <v>330</v>
+      <c r="B234" t="s">
+        <v>328</v>
       </c>
       <c r="C234">
         <f t="shared" si="3"/>
@@ -8112,8 +8109,8 @@
       <c r="A235">
         <v>233</v>
       </c>
-      <c r="B235" s="12" t="s">
-        <v>131</v>
+      <c r="B235" t="s">
+        <v>129</v>
       </c>
       <c r="C235">
         <f t="shared" si="3"/>
@@ -8124,8 +8121,8 @@
       <c r="A236">
         <v>234</v>
       </c>
-      <c r="B236" s="12" t="s">
-        <v>331</v>
+      <c r="B236" t="s">
+        <v>329</v>
       </c>
       <c r="C236">
         <f t="shared" si="3"/>
@@ -8136,7 +8133,7 @@
       <c r="A237">
         <v>235</v>
       </c>
-      <c r="B237" s="12" t="s">
+      <c r="B237" t="s">
         <v>96</v>
       </c>
       <c r="C237">
@@ -8148,8 +8145,8 @@
       <c r="A238">
         <v>236</v>
       </c>
-      <c r="B238" s="12" t="s">
-        <v>332</v>
+      <c r="B238" t="s">
+        <v>330</v>
       </c>
       <c r="C238">
         <f t="shared" si="3"/>
@@ -8160,8 +8157,8 @@
       <c r="A239">
         <v>237</v>
       </c>
-      <c r="B239" s="12" t="s">
-        <v>333</v>
+      <c r="B239" t="s">
+        <v>331</v>
       </c>
       <c r="C239">
         <f t="shared" si="3"/>
@@ -8172,7 +8169,7 @@
       <c r="A240">
         <v>238</v>
       </c>
-      <c r="B240" s="12" t="s">
+      <c r="B240" t="s">
         <v>104</v>
       </c>
       <c r="C240">
@@ -8184,8 +8181,8 @@
       <c r="A241">
         <v>239</v>
       </c>
-      <c r="B241" s="12" t="s">
-        <v>334</v>
+      <c r="B241" t="s">
+        <v>332</v>
       </c>
       <c r="C241">
         <f t="shared" si="3"/>
@@ -8196,7 +8193,7 @@
       <c r="A242">
         <v>240</v>
       </c>
-      <c r="B242" s="12" t="s">
+      <c r="B242" t="s">
         <v>84</v>
       </c>
       <c r="C242">
@@ -8208,8 +8205,8 @@
       <c r="A243">
         <v>241</v>
       </c>
-      <c r="B243" s="12" t="s">
-        <v>335</v>
+      <c r="B243" t="s">
+        <v>333</v>
       </c>
       <c r="C243">
         <f t="shared" si="3"/>
@@ -8220,8 +8217,8 @@
       <c r="A244">
         <v>242</v>
       </c>
-      <c r="B244" s="12" t="s">
-        <v>336</v>
+      <c r="B244" t="s">
+        <v>334</v>
       </c>
       <c r="C244">
         <f t="shared" si="3"/>
@@ -8232,7 +8229,7 @@
       <c r="A245">
         <v>243</v>
       </c>
-      <c r="B245" s="12" t="s">
+      <c r="B245" t="s">
         <v>95</v>
       </c>
       <c r="C245">
@@ -8244,8 +8241,8 @@
       <c r="A246">
         <v>244</v>
       </c>
-      <c r="B246" s="12" t="s">
-        <v>337</v>
+      <c r="B246" t="s">
+        <v>335</v>
       </c>
       <c r="C246">
         <f t="shared" si="3"/>
@@ -8256,8 +8253,8 @@
       <c r="A247">
         <v>245</v>
       </c>
-      <c r="B247" s="12" t="s">
-        <v>338</v>
+      <c r="B247" t="s">
+        <v>336</v>
       </c>
       <c r="C247">
         <f t="shared" si="3"/>
@@ -8268,8 +8265,8 @@
       <c r="A248">
         <v>246</v>
       </c>
-      <c r="B248" s="12" t="s">
-        <v>339</v>
+      <c r="B248" t="s">
+        <v>337</v>
       </c>
       <c r="C248">
         <f t="shared" si="3"/>
@@ -8280,8 +8277,8 @@
       <c r="A249">
         <v>247</v>
       </c>
-      <c r="B249" s="12" t="s">
-        <v>138</v>
+      <c r="B249" t="s">
+        <v>136</v>
       </c>
       <c r="C249">
         <f t="shared" si="3"/>
@@ -8292,7 +8289,7 @@
       <c r="A250">
         <v>248</v>
       </c>
-      <c r="B250" s="12" t="s">
+      <c r="B250" t="s">
         <v>86</v>
       </c>
       <c r="C250">
@@ -8304,8 +8301,8 @@
       <c r="A251">
         <v>249</v>
       </c>
-      <c r="B251" s="12" t="s">
-        <v>340</v>
+      <c r="B251" t="s">
+        <v>338</v>
       </c>
       <c r="C251">
         <f t="shared" si="3"/>
@@ -8316,8 +8313,8 @@
       <c r="A252">
         <v>250</v>
       </c>
-      <c r="B252" s="12" t="s">
-        <v>341</v>
+      <c r="B252" t="s">
+        <v>339</v>
       </c>
       <c r="C252">
         <f t="shared" si="3"/>
@@ -8328,7 +8325,7 @@
       <c r="A253">
         <v>251</v>
       </c>
-      <c r="B253" s="12" t="s">
+      <c r="B253" t="s">
         <v>98</v>
       </c>
       <c r="C253">
@@ -8340,8 +8337,8 @@
       <c r="A254">
         <v>252</v>
       </c>
-      <c r="B254" s="12" t="s">
-        <v>342</v>
+      <c r="B254" t="s">
+        <v>340</v>
       </c>
       <c r="C254">
         <f t="shared" si="3"/>
@@ -8352,7 +8349,7 @@
       <c r="A255">
         <v>253</v>
       </c>
-      <c r="B255" s="12" t="s">
+      <c r="B255" t="s">
         <v>74</v>
       </c>
       <c r="C255">
@@ -8364,8 +8361,8 @@
       <c r="A256">
         <v>254</v>
       </c>
-      <c r="B256" s="12" t="s">
-        <v>320</v>
+      <c r="B256" t="s">
+        <v>318</v>
       </c>
       <c r="C256">
         <f t="shared" si="3"/>
@@ -8376,8 +8373,8 @@
       <c r="A257">
         <v>255</v>
       </c>
-      <c r="B257" s="12" t="s">
-        <v>343</v>
+      <c r="B257" t="s">
+        <v>341</v>
       </c>
       <c r="C257">
         <f t="shared" si="3"/>
@@ -8388,7 +8385,7 @@
       <c r="A258">
         <v>256</v>
       </c>
-      <c r="B258" s="12" t="s">
+      <c r="B258" t="s">
         <v>88</v>
       </c>
       <c r="C258">
@@ -8400,8 +8397,8 @@
       <c r="A259">
         <v>257</v>
       </c>
-      <c r="B259" s="12" t="s">
-        <v>344</v>
+      <c r="B259" t="s">
+        <v>342</v>
       </c>
       <c r="C259">
         <f t="shared" si="4"/>
@@ -8412,8 +8409,8 @@
       <c r="A260">
         <v>258</v>
       </c>
-      <c r="B260" s="12" t="s">
-        <v>345</v>
+      <c r="B260" t="s">
+        <v>343</v>
       </c>
       <c r="C260">
         <f t="shared" si="4"/>
@@ -8424,7 +8421,7 @@
       <c r="A261">
         <v>259</v>
       </c>
-      <c r="B261" s="12" t="s">
+      <c r="B261" t="s">
         <v>97</v>
       </c>
       <c r="C261">
@@ -8436,8 +8433,8 @@
       <c r="A262">
         <v>260</v>
       </c>
-      <c r="B262" s="12" t="s">
-        <v>346</v>
+      <c r="B262" t="s">
+        <v>344</v>
       </c>
       <c r="C262">
         <f t="shared" si="4"/>
@@ -8448,7 +8445,7 @@
       <c r="A263">
         <v>261</v>
       </c>
-      <c r="B263" s="12" t="s">
+      <c r="B263" t="s">
         <v>73</v>
       </c>
       <c r="C263">
@@ -8460,8 +8457,8 @@
       <c r="A264">
         <v>262</v>
       </c>
-      <c r="B264" s="12" t="s">
-        <v>347</v>
+      <c r="B264" t="s">
+        <v>345</v>
       </c>
       <c r="C264">
         <f t="shared" si="4"/>
@@ -8472,8 +8469,8 @@
       <c r="A265">
         <v>263</v>
       </c>
-      <c r="B265" s="12" t="s">
-        <v>348</v>
+      <c r="B265" t="s">
+        <v>346</v>
       </c>
       <c r="C265">
         <f t="shared" si="4"/>
@@ -8484,7 +8481,7 @@
       <c r="A266">
         <v>264</v>
       </c>
-      <c r="B266" s="12" t="s">
+      <c r="B266" t="s">
         <v>89</v>
       </c>
       <c r="C266">
@@ -8496,8 +8493,8 @@
       <c r="A267">
         <v>265</v>
       </c>
-      <c r="B267" s="12" t="s">
-        <v>349</v>
+      <c r="B267" t="s">
+        <v>347</v>
       </c>
       <c r="C267">
         <f t="shared" si="4"/>
@@ -8508,7 +8505,7 @@
       <c r="A268">
         <v>266</v>
       </c>
-      <c r="B268" s="12" t="s">
+      <c r="B268" t="s">
         <v>64</v>
       </c>
       <c r="C268">
@@ -8520,7 +8517,7 @@
       <c r="A269">
         <v>267</v>
       </c>
-      <c r="B269" s="12" t="s">
+      <c r="B269" t="s">
         <v>100</v>
       </c>
       <c r="C269">
@@ -8532,8 +8529,8 @@
       <c r="A270">
         <v>268</v>
       </c>
-      <c r="B270" s="12" t="s">
-        <v>350</v>
+      <c r="B270" t="s">
+        <v>348</v>
       </c>
       <c r="C270">
         <f t="shared" si="4"/>
@@ -8544,7 +8541,7 @@
       <c r="A271">
         <v>269</v>
       </c>
-      <c r="B271" s="12" t="s">
+      <c r="B271" t="s">
         <v>75</v>
       </c>
       <c r="C271">
@@ -8556,8 +8553,8 @@
       <c r="A272">
         <v>270</v>
       </c>
-      <c r="B272" s="12" t="s">
-        <v>351</v>
+      <c r="B272" t="s">
+        <v>349</v>
       </c>
       <c r="C272">
         <f t="shared" si="4"/>
@@ -8568,7 +8565,7 @@
       <c r="A273">
         <v>271</v>
       </c>
-      <c r="B273" s="12" t="s">
+      <c r="B273" t="s">
         <v>53</v>
       </c>
       <c r="C273">
@@ -8580,7 +8577,7 @@
       <c r="A274">
         <v>272</v>
       </c>
-      <c r="B274" s="12" t="s">
+      <c r="B274" t="s">
         <v>91</v>
       </c>
       <c r="C274">
@@ -8592,8 +8589,8 @@
       <c r="A275">
         <v>273</v>
       </c>
-      <c r="B275" s="12" t="s">
-        <v>307</v>
+      <c r="B275" t="s">
+        <v>305</v>
       </c>
       <c r="C275">
         <f t="shared" si="4"/>
@@ -8604,7 +8601,7 @@
       <c r="A276">
         <v>274</v>
       </c>
-      <c r="B276" s="12" t="s">
+      <c r="B276" t="s">
         <v>70</v>
       </c>
       <c r="C276">
@@ -8616,8 +8613,8 @@
       <c r="A277">
         <v>275</v>
       </c>
-      <c r="B277" s="12" t="s">
-        <v>352</v>
+      <c r="B277" t="s">
+        <v>350</v>
       </c>
       <c r="C277">
         <f t="shared" si="4"/>
@@ -8628,8 +8625,8 @@
       <c r="A278">
         <v>276</v>
       </c>
-      <c r="B278" s="12" t="s">
-        <v>353</v>
+      <c r="B278" t="s">
+        <v>351</v>
       </c>
       <c r="C278">
         <f t="shared" si="4"/>
@@ -8640,7 +8637,7 @@
       <c r="A279">
         <v>277</v>
       </c>
-      <c r="B279" s="12" t="s">
+      <c r="B279" t="s">
         <v>79</v>
       </c>
       <c r="C279">
@@ -8652,8 +8649,8 @@
       <c r="A280">
         <v>278</v>
       </c>
-      <c r="B280" s="12" t="s">
-        <v>354</v>
+      <c r="B280" t="s">
+        <v>352</v>
       </c>
       <c r="C280">
         <f t="shared" si="4"/>
@@ -8664,7 +8661,7 @@
       <c r="A281">
         <v>279</v>
       </c>
-      <c r="B281" s="12" t="s">
+      <c r="B281" t="s">
         <v>56</v>
       </c>
       <c r="C281">
@@ -8676,7 +8673,7 @@
       <c r="A282">
         <v>280</v>
       </c>
-      <c r="B282" s="12" t="s">
+      <c r="B282" t="s">
         <v>90</v>
       </c>
       <c r="C282">
@@ -8688,8 +8685,8 @@
       <c r="A283">
         <v>281</v>
       </c>
-      <c r="B283" s="12" t="s">
-        <v>355</v>
+      <c r="B283" t="s">
+        <v>353</v>
       </c>
       <c r="C283">
         <f t="shared" si="4"/>
@@ -8700,7 +8697,7 @@
       <c r="A284">
         <v>282</v>
       </c>
-      <c r="B284" s="12" t="s">
+      <c r="B284" t="s">
         <v>65</v>
       </c>
       <c r="C284">
@@ -8712,7 +8709,7 @@
       <c r="A285">
         <v>283</v>
       </c>
-      <c r="B285" s="12" t="s">
+      <c r="B285" t="s">
         <v>103</v>
       </c>
       <c r="C285">
@@ -8724,7 +8721,7 @@
       <c r="A286">
         <v>284</v>
       </c>
-      <c r="B286" s="12" t="s">
+      <c r="B286" t="s">
         <v>40</v>
       </c>
       <c r="C286">
@@ -8736,7 +8733,7 @@
       <c r="A287">
         <v>285</v>
       </c>
-      <c r="B287" s="12" t="s">
+      <c r="B287" t="s">
         <v>75</v>
       </c>
       <c r="C287">
@@ -8748,8 +8745,8 @@
       <c r="A288">
         <v>286</v>
       </c>
-      <c r="B288" s="12" t="s">
-        <v>356</v>
+      <c r="B288" t="s">
+        <v>354</v>
       </c>
       <c r="C288">
         <f t="shared" si="4"/>
@@ -8760,7 +8757,7 @@
       <c r="A289">
         <v>287</v>
       </c>
-      <c r="B289" s="12" t="s">
+      <c r="B289" t="s">
         <v>50</v>
       </c>
       <c r="C289">
@@ -8772,7 +8769,7 @@
       <c r="A290">
         <v>288</v>
       </c>
-      <c r="B290" s="12" t="s">
+      <c r="B290" t="s">
         <v>87</v>
       </c>
       <c r="C290">
@@ -8784,8 +8781,8 @@
       <c r="A291">
         <v>289</v>
       </c>
-      <c r="B291" s="12" t="s">
-        <v>357</v>
+      <c r="B291" t="s">
+        <v>355</v>
       </c>
       <c r="C291">
         <f t="shared" si="4"/>
@@ -8796,7 +8793,7 @@
       <c r="A292">
         <v>290</v>
       </c>
-      <c r="B292" s="12" t="s">
+      <c r="B292" t="s">
         <v>63</v>
       </c>
       <c r="C292">
@@ -8808,7 +8805,7 @@
       <c r="A293">
         <v>291</v>
       </c>
-      <c r="B293" s="12" t="s">
+      <c r="B293" t="s">
         <v>100</v>
       </c>
       <c r="C293">
@@ -8820,7 +8817,7 @@
       <c r="A294">
         <v>292</v>
       </c>
-      <c r="B294" s="12" t="s">
+      <c r="B294" t="s">
         <v>39</v>
       </c>
       <c r="C294">
@@ -8832,7 +8829,7 @@
       <c r="A295">
         <v>293</v>
       </c>
-      <c r="B295" s="12" t="s">
+      <c r="B295" t="s">
         <v>72</v>
       </c>
       <c r="C295">
@@ -8844,8 +8841,8 @@
       <c r="A296">
         <v>294</v>
       </c>
-      <c r="B296" s="12" t="s">
-        <v>358</v>
+      <c r="B296" t="s">
+        <v>356</v>
       </c>
       <c r="C296">
         <f t="shared" si="4"/>
@@ -8856,7 +8853,7 @@
       <c r="A297">
         <v>295</v>
       </c>
-      <c r="B297" s="12" t="s">
+      <c r="B297" t="s">
         <v>48</v>
       </c>
       <c r="C297">
@@ -8868,7 +8865,7 @@
       <c r="A298">
         <v>296</v>
       </c>
-      <c r="B298" s="12" t="s">
+      <c r="B298" t="s">
         <v>85</v>
       </c>
       <c r="C298">
@@ -8880,7 +8877,7 @@
       <c r="A299">
         <v>297</v>
       </c>
-      <c r="B299" s="12" t="s">
+      <c r="B299" t="s">
         <v>31</v>
       </c>
       <c r="C299">
@@ -8892,7 +8889,7 @@
       <c r="A300">
         <v>298</v>
       </c>
-      <c r="B300" s="12" t="s">
+      <c r="B300" t="s">
         <v>61</v>
       </c>
       <c r="C300">
@@ -8904,7 +8901,7 @@
       <c r="A301">
         <v>299</v>
       </c>
-      <c r="B301" s="12" t="s">
+      <c r="B301" t="s">
         <v>99</v>
       </c>
       <c r="C301">
@@ -8916,7 +8913,7 @@
       <c r="A302">
         <v>300</v>
       </c>
-      <c r="B302" s="12" t="s">
+      <c r="B302" t="s">
         <v>42</v>
       </c>
       <c r="C302">
@@ -8928,7 +8925,7 @@
       <c r="A303">
         <v>301</v>
       </c>
-      <c r="B303" s="12" t="s">
+      <c r="B303" t="s">
         <v>76</v>
       </c>
       <c r="C303">
@@ -8940,7 +8937,7 @@
       <c r="A304">
         <v>302</v>
       </c>
-      <c r="B304" s="12" t="s">
+      <c r="B304" t="s">
         <v>27</v>
       </c>
       <c r="C304">
@@ -8952,7 +8949,7 @@
       <c r="A305">
         <v>303</v>
       </c>
-      <c r="B305" s="12" t="s">
+      <c r="B305" t="s">
         <v>55</v>
       </c>
       <c r="C305">
@@ -8964,7 +8961,7 @@
       <c r="A306">
         <v>304</v>
       </c>
-      <c r="B306" s="12" t="s">
+      <c r="B306" t="s">
         <v>90</v>
       </c>
       <c r="C306">
@@ -8976,7 +8973,7 @@
       <c r="A307">
         <v>305</v>
       </c>
-      <c r="B307" s="12" t="s">
+      <c r="B307" t="s">
         <v>38</v>
       </c>
       <c r="C307">
@@ -8988,7 +8985,7 @@
       <c r="A308">
         <v>306</v>
       </c>
-      <c r="B308" s="12" t="s">
+      <c r="B308" t="s">
         <v>69</v>
       </c>
       <c r="C308">
@@ -9000,7 +8997,7 @@
       <c r="A309">
         <v>307</v>
       </c>
-      <c r="B309" s="12" t="s">
+      <c r="B309" t="s">
         <v>101</v>
       </c>
       <c r="C309">
@@ -9012,7 +9009,7 @@
       <c r="A310">
         <v>308</v>
       </c>
-      <c r="B310" s="12" t="s">
+      <c r="B310" t="s">
         <v>47</v>
       </c>
       <c r="C310">
@@ -9024,7 +9021,7 @@
       <c r="A311">
         <v>309</v>
       </c>
-      <c r="B311" s="12" t="s">
+      <c r="B311" t="s">
         <v>82</v>
       </c>
       <c r="C311">
@@ -9036,7 +9033,7 @@
       <c r="A312">
         <v>310</v>
       </c>
-      <c r="B312" s="12" t="s">
+      <c r="B312" t="s">
         <v>32</v>
       </c>
       <c r="C312">
@@ -9048,7 +9045,7 @@
       <c r="A313">
         <v>311</v>
       </c>
-      <c r="B313" s="12" t="s">
+      <c r="B313" t="s">
         <v>60</v>
       </c>
       <c r="C313">
@@ -9060,7 +9057,7 @@
       <c r="A314">
         <v>312</v>
       </c>
-      <c r="B314" s="12" t="s">
+      <c r="B314" t="s">
         <v>94</v>
       </c>
       <c r="C314">
@@ -9072,7 +9069,7 @@
       <c r="A315">
         <v>313</v>
       </c>
-      <c r="B315" s="12" t="s">
+      <c r="B315" t="s">
         <v>38</v>
       </c>
       <c r="C315">
@@ -9084,7 +9081,7 @@
       <c r="A316">
         <v>314</v>
       </c>
-      <c r="B316" s="12" t="s">
+      <c r="B316" t="s">
         <v>68</v>
       </c>
       <c r="C316">
@@ -9096,7 +9093,7 @@
       <c r="A317">
         <v>315</v>
       </c>
-      <c r="B317" s="12" t="s">
+      <c r="B317" t="s">
         <v>21</v>
       </c>
       <c r="C317">
@@ -9108,7 +9105,7 @@
       <c r="A318">
         <v>316</v>
       </c>
-      <c r="B318" s="12" t="s">
+      <c r="B318" t="s">
         <v>46</v>
       </c>
       <c r="C318">
@@ -9120,7 +9117,7 @@
       <c r="A319">
         <v>317</v>
       </c>
-      <c r="B319" s="12" t="s">
+      <c r="B319" t="s">
         <v>81</v>
       </c>
       <c r="C319">
@@ -9132,7 +9129,7 @@
       <c r="A320">
         <v>318</v>
       </c>
-      <c r="B320" s="12" t="s">
+      <c r="B320" t="s">
         <v>25</v>
       </c>
       <c r="C320">
@@ -9144,7 +9141,7 @@
       <c r="A321">
         <v>319</v>
       </c>
-      <c r="B321" s="12" t="s">
+      <c r="B321" t="s">
         <v>58</v>
       </c>
       <c r="C321">
@@ -9156,7 +9153,7 @@
       <c r="A322">
         <v>320</v>
       </c>
-      <c r="B322" s="12" t="s">
+      <c r="B322" t="s">
         <v>80</v>
       </c>
       <c r="C322">
@@ -9168,7 +9165,7 @@
       <c r="A323">
         <v>321</v>
       </c>
-      <c r="B323" s="12" t="s">
+      <c r="B323" t="s">
         <v>36</v>
       </c>
       <c r="C323">
@@ -9180,7 +9177,7 @@
       <c r="A324">
         <v>322</v>
       </c>
-      <c r="B324" s="12" t="s">
+      <c r="B324" t="s">
         <v>64</v>
       </c>
       <c r="C324">
@@ -9192,7 +9189,7 @@
       <c r="A325">
         <v>323</v>
       </c>
-      <c r="B325" s="12" t="s">
+      <c r="B325" t="s">
         <v>20</v>
       </c>
       <c r="C325">
@@ -9204,7 +9201,7 @@
       <c r="A326">
         <v>324</v>
       </c>
-      <c r="B326" s="12" t="s">
+      <c r="B326" t="s">
         <v>41</v>
       </c>
       <c r="C326">
@@ -9216,7 +9213,7 @@
       <c r="A327">
         <v>325</v>
       </c>
-      <c r="B327" s="12" t="s">
+      <c r="B327" t="s">
         <v>77</v>
       </c>
       <c r="C327">
@@ -9228,7 +9225,7 @@
       <c r="A328">
         <v>326</v>
       </c>
-      <c r="B328" s="12" t="s">
+      <c r="B328" t="s">
         <v>28</v>
       </c>
       <c r="C328">
@@ -9240,7 +9237,7 @@
       <c r="A329">
         <v>327</v>
       </c>
-      <c r="B329" s="12" t="s">
+      <c r="B329" t="s">
         <v>51</v>
       </c>
       <c r="C329">
@@ -9252,7 +9249,7 @@
       <c r="A330">
         <v>328</v>
       </c>
-      <c r="B330" s="12" t="s">
+      <c r="B330" t="s">
         <v>17</v>
       </c>
       <c r="C330">
@@ -9264,7 +9261,7 @@
       <c r="A331">
         <v>329</v>
       </c>
-      <c r="B331" s="12" t="s">
+      <c r="B331" t="s">
         <v>37</v>
       </c>
       <c r="C331">
@@ -9276,7 +9273,7 @@
       <c r="A332">
         <v>330</v>
       </c>
-      <c r="B332" s="12" t="s">
+      <c r="B332" t="s">
         <v>67</v>
       </c>
       <c r="C332">
@@ -9288,7 +9285,7 @@
       <c r="A333">
         <v>331</v>
       </c>
-      <c r="B333" s="12" t="s">
+      <c r="B333" t="s">
         <v>22</v>
       </c>
       <c r="C333">
@@ -9300,7 +9297,7 @@
       <c r="A334">
         <v>332</v>
       </c>
-      <c r="B334" s="12" t="s">
+      <c r="B334" t="s">
         <v>43</v>
       </c>
       <c r="C334">
@@ -9312,7 +9309,7 @@
       <c r="A335">
         <v>333</v>
       </c>
-      <c r="B335" s="12" t="s">
+      <c r="B335" t="s">
         <v>25</v>
       </c>
       <c r="C335">
@@ -9324,7 +9321,7 @@
       <c r="A336">
         <v>334</v>
       </c>
-      <c r="B336" s="12" t="s">
+      <c r="B336" t="s">
         <v>29</v>
       </c>
       <c r="C336">
@@ -9336,7 +9333,7 @@
       <c r="A337">
         <v>335</v>
       </c>
-      <c r="B337" s="12" t="s">
+      <c r="B337" t="s">
         <v>54</v>
       </c>
       <c r="C337">
@@ -9348,7 +9345,7 @@
       <c r="A338">
         <v>336</v>
       </c>
-      <c r="B338" s="12" t="s">
+      <c r="B338" t="s">
         <v>12</v>
       </c>
       <c r="C338">
@@ -9360,7 +9357,7 @@
       <c r="A339">
         <v>337</v>
       </c>
-      <c r="B339" s="12" t="s">
+      <c r="B339" t="s">
         <v>34</v>
       </c>
       <c r="C339">
@@ -9372,7 +9369,7 @@
       <c r="A340">
         <v>338</v>
       </c>
-      <c r="B340" s="12" t="s">
+      <c r="B340" t="s">
         <v>66</v>
       </c>
       <c r="C340">
@@ -9384,7 +9381,7 @@
       <c r="A341">
         <v>339</v>
       </c>
-      <c r="B341" s="12" t="s">
+      <c r="B341" t="s">
         <v>16</v>
       </c>
       <c r="C341">
@@ -9396,7 +9393,7 @@
       <c r="A342">
         <v>340</v>
       </c>
-      <c r="B342" s="12" t="s">
+      <c r="B342" t="s">
         <v>40</v>
       </c>
       <c r="C342">
@@ -9408,7 +9405,7 @@
       <c r="A343">
         <v>341</v>
       </c>
-      <c r="B343" s="12" t="s">
+      <c r="B343" t="s">
         <v>10</v>
       </c>
       <c r="C343">
@@ -9420,7 +9417,7 @@
       <c r="A344">
         <v>342</v>
       </c>
-      <c r="B344" s="12" t="s">
+      <c r="B344" t="s">
         <v>30</v>
       </c>
       <c r="C344">
@@ -9432,7 +9429,7 @@
       <c r="A345">
         <v>343</v>
       </c>
-      <c r="B345" s="12" t="s">
+      <c r="B345" t="s">
         <v>57</v>
       </c>
       <c r="C345">
@@ -9444,7 +9441,7 @@
       <c r="A346">
         <v>344</v>
       </c>
-      <c r="B346" s="12" t="s">
+      <c r="B346" t="s">
         <v>13</v>
       </c>
       <c r="C346">
@@ -9456,7 +9453,7 @@
       <c r="A347">
         <v>345</v>
       </c>
-      <c r="B347" s="12" t="s">
+      <c r="B347" t="s">
         <v>35</v>
       </c>
       <c r="C347">
@@ -9468,7 +9465,7 @@
       <c r="A348">
         <v>346</v>
       </c>
-      <c r="B348" s="12" t="s">
+      <c r="B348" t="s">
         <v>3</v>
       </c>
       <c r="C348">
@@ -9480,7 +9477,7 @@
       <c r="A349">
         <v>347</v>
       </c>
-      <c r="B349" s="12" t="s">
+      <c r="B349" t="s">
         <v>19</v>
       </c>
       <c r="C349">
@@ -9492,7 +9489,7 @@
       <c r="A350">
         <v>348</v>
       </c>
-      <c r="B350" s="12" t="s">
+      <c r="B350" t="s">
         <v>45</v>
       </c>
       <c r="C350">
@@ -9504,7 +9501,7 @@
       <c r="A351">
         <v>349</v>
       </c>
-      <c r="B351" s="12" t="s">
+      <c r="B351" t="s">
         <v>7</v>
       </c>
       <c r="C351">
@@ -9516,7 +9513,7 @@
       <c r="A352">
         <v>350</v>
       </c>
-      <c r="B352" s="12" t="s">
+      <c r="B352" t="s">
         <v>24</v>
       </c>
       <c r="C352">
@@ -9528,7 +9525,7 @@
       <c r="A353">
         <v>351</v>
       </c>
-      <c r="B353" s="12" t="s">
+      <c r="B353" t="s">
         <v>52</v>
       </c>
       <c r="C353">
@@ -9540,7 +9537,7 @@
       <c r="A354">
         <v>352</v>
       </c>
-      <c r="B354" s="12" t="s">
+      <c r="B354" t="s">
         <v>15</v>
       </c>
       <c r="C354">
@@ -9552,7 +9549,7 @@
       <c r="A355">
         <v>353</v>
       </c>
-      <c r="B355" s="12" t="s">
+      <c r="B355" t="s">
         <v>36</v>
       </c>
       <c r="C355">
@@ -9564,7 +9561,7 @@
       <c r="A356">
         <v>354</v>
       </c>
-      <c r="B356" s="12" t="s">
+      <c r="B356" t="s">
         <v>6</v>
       </c>
       <c r="C356">
@@ -9576,7 +9573,7 @@
       <c r="A357">
         <v>355</v>
       </c>
-      <c r="B357" s="12" t="s">
+      <c r="B357" t="s">
         <v>18</v>
       </c>
       <c r="C357">
@@ -9588,7 +9585,7 @@
       <c r="A358">
         <v>356</v>
       </c>
-      <c r="B358" s="12" t="s">
+      <c r="B358" t="s">
         <v>43</v>
       </c>
       <c r="C358">
@@ -9600,7 +9597,7 @@
       <c r="A359">
         <v>357</v>
       </c>
-      <c r="B359" s="12" t="s">
+      <c r="B359" t="s">
         <v>7</v>
       </c>
       <c r="C359">
@@ -9612,7 +9609,7 @@
       <c r="A360">
         <v>358</v>
       </c>
-      <c r="B360" s="12" t="s">
+      <c r="B360" t="s">
         <v>29</v>
       </c>
       <c r="C360">
@@ -9624,7 +9621,7 @@
       <c r="A361">
         <v>359</v>
       </c>
-      <c r="B361" s="12" t="s">
+      <c r="B361" t="s">
         <v>1</v>
       </c>
       <c r="C361">
@@ -9636,7 +9633,7 @@
       <c r="A362">
         <v>360</v>
       </c>
-      <c r="B362" s="12" t="s">
+      <c r="B362" t="s">
         <v>13</v>
       </c>
       <c r="C362">
@@ -9648,7 +9645,7 @@
       <c r="A363">
         <v>361</v>
       </c>
-      <c r="B363" s="12" t="s">
+      <c r="B363" t="s">
         <v>36</v>
       </c>
       <c r="C363">
@@ -9660,7 +9657,7 @@
       <c r="A364">
         <v>362</v>
       </c>
-      <c r="B364" s="12" t="s">
+      <c r="B364" t="s">
         <v>1</v>
       </c>
       <c r="C364">
@@ -9672,7 +9669,7 @@
       <c r="A365">
         <v>363</v>
       </c>
-      <c r="B365" s="12" t="s">
+      <c r="B365" t="s">
         <v>14</v>
       </c>
       <c r="C365">
@@ -9684,7 +9681,7 @@
       <c r="A366">
         <v>364</v>
       </c>
-      <c r="B366" s="12" t="s">
+      <c r="B366" t="s">
         <v>11</v>
       </c>
       <c r="C366">
@@ -9696,7 +9693,7 @@
       <c r="A367">
         <v>365</v>
       </c>
-      <c r="B367" s="12" t="s">
+      <c r="B367" t="s">
         <v>5</v>
       </c>
       <c r="C367">
@@ -9708,7 +9705,7 @@
       <c r="A368">
         <v>366</v>
       </c>
-      <c r="B368" s="12" t="s">
+      <c r="B368" t="s">
         <v>20</v>
       </c>
       <c r="C368">
@@ -9720,7 +9717,7 @@
       <c r="A369">
         <v>367</v>
       </c>
-      <c r="B369" s="12" t="s">
+      <c r="B369" t="s">
         <v>3</v>
       </c>
       <c r="C369">
@@ -9732,7 +9729,7 @@
       <c r="A370">
         <v>368</v>
       </c>
-      <c r="B370" s="12" t="s">
+      <c r="B370" t="s">
         <v>13</v>
       </c>
       <c r="C370">
@@ -9744,7 +9741,7 @@
       <c r="A371">
         <v>369</v>
       </c>
-      <c r="B371" s="12" t="s">
+      <c r="B371" t="s">
         <v>35</v>
       </c>
       <c r="C371">
@@ -9756,7 +9753,7 @@
       <c r="A372">
         <v>370</v>
       </c>
-      <c r="B372" s="12" t="s">
+      <c r="B372" t="s">
         <v>7</v>
       </c>
       <c r="C372">
@@ -9768,7 +9765,7 @@
       <c r="A373">
         <v>371</v>
       </c>
-      <c r="B373" s="12" t="s">
+      <c r="B373" t="s">
         <v>20</v>
       </c>
       <c r="C373">
@@ -9780,7 +9777,7 @@
       <c r="A374">
         <v>372</v>
       </c>
-      <c r="B374" s="12" t="s">
+      <c r="B374" t="s">
         <v>1</v>
       </c>
       <c r="C374">
@@ -9792,7 +9789,7 @@
       <c r="A375">
         <v>373</v>
       </c>
-      <c r="B375" s="12" t="s">
+      <c r="B375" t="s">
         <v>8</v>
       </c>
       <c r="C375">
@@ -9804,7 +9801,7 @@
       <c r="A376">
         <v>374</v>
       </c>
-      <c r="B376" s="12" t="s">
+      <c r="B376" t="s">
         <v>26</v>
       </c>
       <c r="C376">
@@ -9816,7 +9813,7 @@
       <c r="A377">
         <v>375</v>
       </c>
-      <c r="B377" s="12" t="s">
+      <c r="B377" t="s">
         <v>1</v>
       </c>
       <c r="C377">
@@ -9828,7 +9825,7 @@
       <c r="A378">
         <v>376</v>
       </c>
-      <c r="B378" s="12" t="s">
+      <c r="B378" t="s">
         <v>10</v>
       </c>
       <c r="C378">
@@ -9840,7 +9837,7 @@
       <c r="A379">
         <v>378</v>
       </c>
-      <c r="B379" s="12" t="s">
+      <c r="B379" t="s">
         <v>4</v>
       </c>
       <c r="C379">
@@ -9852,7 +9849,7 @@
       <c r="A380">
         <v>379</v>
       </c>
-      <c r="B380" s="12" t="s">
+      <c r="B380" t="s">
         <v>22</v>
       </c>
       <c r="C380">
@@ -9864,7 +9861,7 @@
       <c r="A381">
         <v>380</v>
       </c>
-      <c r="B381" s="12" t="s">
+      <c r="B381" t="s">
         <v>0</v>
       </c>
       <c r="C381">
@@ -9876,7 +9873,7 @@
       <c r="A382">
         <v>381</v>
       </c>
-      <c r="B382" s="12" t="s">
+      <c r="B382" t="s">
         <v>9</v>
       </c>
       <c r="C382">
@@ -9888,7 +9885,7 @@
       <c r="A383">
         <v>382</v>
       </c>
-      <c r="B383" s="12" t="s">
+      <c r="B383" t="s">
         <v>30</v>
       </c>
       <c r="C383">
@@ -9900,7 +9897,7 @@
       <c r="A384">
         <v>383</v>
       </c>
-      <c r="B384" s="12" t="s">
+      <c r="B384" t="s">
         <v>2</v>
       </c>
       <c r="C384">
@@ -9912,7 +9909,7 @@
       <c r="A385">
         <v>384</v>
       </c>
-      <c r="B385" s="12" t="s">
+      <c r="B385" t="s">
         <v>13</v>
       </c>
       <c r="C385">
@@ -9924,11 +9921,11 @@
       <c r="A386">
         <v>385</v>
       </c>
-      <c r="B386" s="12" t="s">
+      <c r="B386" t="s">
         <v>0</v>
       </c>
       <c r="C386">
-        <f t="shared" ref="C386:C449" si="6">VALUE(MID(B386, FIND("(", B386) + 1, FIND(")", B386) - FIND("(", B386) - 1))</f>
+        <f t="shared" ref="C386:C438" si="6">VALUE(MID(B386, FIND("(", B386) + 1, FIND(")", B386) - FIND("(", B386) - 1))</f>
         <v>1</v>
       </c>
     </row>
@@ -9936,7 +9933,7 @@
       <c r="A387">
         <v>386</v>
       </c>
-      <c r="B387" s="12" t="s">
+      <c r="B387" t="s">
         <v>7</v>
       </c>
       <c r="C387">
@@ -9948,7 +9945,7 @@
       <c r="A388">
         <v>387</v>
       </c>
-      <c r="B388" s="12" t="s">
+      <c r="B388" t="s">
         <v>21</v>
       </c>
       <c r="C388">
@@ -9960,7 +9957,7 @@
       <c r="A389">
         <v>388</v>
       </c>
-      <c r="B389" s="12" t="s">
+      <c r="B389" t="s">
         <v>2</v>
       </c>
       <c r="C389">
@@ -9972,7 +9969,7 @@
       <c r="A390">
         <v>389</v>
       </c>
-      <c r="B390" s="12" t="s">
+      <c r="B390" t="s">
         <v>6</v>
       </c>
       <c r="C390">
@@ -9984,7 +9981,7 @@
       <c r="A391">
         <v>391</v>
       </c>
-      <c r="B391" s="12" t="s">
+      <c r="B391" t="s">
         <v>1</v>
       </c>
       <c r="C391">
@@ -9996,7 +9993,7 @@
       <c r="A392">
         <v>392</v>
       </c>
-      <c r="B392" s="12" t="s">
+      <c r="B392" t="s">
         <v>10</v>
       </c>
       <c r="C392">
@@ -10008,7 +10005,7 @@
       <c r="A393">
         <v>394</v>
       </c>
-      <c r="B393" s="12" t="s">
+      <c r="B393" t="s">
         <v>2</v>
       </c>
       <c r="C393">
@@ -10020,7 +10017,7 @@
       <c r="A394">
         <v>395</v>
       </c>
-      <c r="B394" s="12" t="s">
+      <c r="B394" t="s">
         <v>5</v>
       </c>
       <c r="C394">
@@ -10032,7 +10029,7 @@
       <c r="A395">
         <v>397</v>
       </c>
-      <c r="B395" s="12" t="s">
+      <c r="B395" t="s">
         <v>2</v>
       </c>
       <c r="C395">
@@ -10044,7 +10041,7 @@
       <c r="A396">
         <v>399</v>
       </c>
-      <c r="B396" s="12" t="s">
+      <c r="B396" t="s">
         <v>0</v>
       </c>
       <c r="C396">
@@ -10056,7 +10053,7 @@
       <c r="A397">
         <v>400</v>
       </c>
-      <c r="B397" s="12" t="s">
+      <c r="B397" t="s">
         <v>8</v>
       </c>
       <c r="C397">
@@ -10068,7 +10065,7 @@
       <c r="A398">
         <v>402</v>
       </c>
-      <c r="B398" s="12" t="s">
+      <c r="B398" t="s">
         <v>2</v>
       </c>
       <c r="C398">
@@ -10080,7 +10077,7 @@
       <c r="A399">
         <v>404</v>
       </c>
-      <c r="B399" s="12" t="s">
+      <c r="B399" t="s">
         <v>1</v>
       </c>
       <c r="C399">
@@ -10092,7 +10089,7 @@
       <c r="A400">
         <v>405</v>
       </c>
-      <c r="B400" s="12" t="s">
+      <c r="B400" t="s">
         <v>7</v>
       </c>
       <c r="C400">
@@ -10104,7 +10101,7 @@
       <c r="A401">
         <v>406</v>
       </c>
-      <c r="B401" s="12" t="s">
+      <c r="B401" t="s">
         <v>1</v>
       </c>
       <c r="C401">
@@ -10116,7 +10113,7 @@
       <c r="A402">
         <v>407</v>
       </c>
-      <c r="B402" s="12" t="s">
+      <c r="B402" t="s">
         <v>4</v>
       </c>
       <c r="C402">
@@ -10128,7 +10125,7 @@
       <c r="A403">
         <v>409</v>
       </c>
-      <c r="B403" s="12" t="s">
+      <c r="B403" t="s">
         <v>0</v>
       </c>
       <c r="C403">
@@ -10140,7 +10137,7 @@
       <c r="A404">
         <v>410</v>
       </c>
-      <c r="B404" s="12" t="s">
+      <c r="B404" t="s">
         <v>5</v>
       </c>
       <c r="C404">
@@ -10152,7 +10149,7 @@
       <c r="A405">
         <v>412</v>
       </c>
-      <c r="B405" s="12" t="s">
+      <c r="B405" t="s">
         <v>1</v>
       </c>
       <c r="C405">
@@ -10164,7 +10161,7 @@
       <c r="A406">
         <v>413</v>
       </c>
-      <c r="B406" s="12" t="s">
+      <c r="B406" t="s">
         <v>8</v>
       </c>
       <c r="C406">
@@ -10176,7 +10173,7 @@
       <c r="A407">
         <v>415</v>
       </c>
-      <c r="B407" s="12" t="s">
+      <c r="B407" t="s">
         <v>2</v>
       </c>
       <c r="C407">
@@ -10188,7 +10185,7 @@
       <c r="A408">
         <v>417</v>
       </c>
-      <c r="B408" s="12" t="s">
+      <c r="B408" t="s">
         <v>0</v>
       </c>
       <c r="C408">
@@ -10200,7 +10197,7 @@
       <c r="A409">
         <v>418</v>
       </c>
-      <c r="B409" s="12" t="s">
+      <c r="B409" t="s">
         <v>4</v>
       </c>
       <c r="C409">
@@ -10212,7 +10209,7 @@
       <c r="A410">
         <v>420</v>
       </c>
-      <c r="B410" s="12" t="s">
+      <c r="B410" t="s">
         <v>1</v>
       </c>
       <c r="C410">
@@ -10224,7 +10221,7 @@
       <c r="A411">
         <v>422</v>
       </c>
-      <c r="B411" s="12" t="s">
+      <c r="B411" t="s">
         <v>0</v>
       </c>
       <c r="C411">
@@ -10236,7 +10233,7 @@
       <c r="A412">
         <v>423</v>
       </c>
-      <c r="B412" s="12" t="s">
+      <c r="B412" t="s">
         <v>4</v>
       </c>
       <c r="C412">
@@ -10248,7 +10245,7 @@
       <c r="A413">
         <v>425</v>
       </c>
-      <c r="B413" s="12" t="s">
+      <c r="B413" t="s">
         <v>1</v>
       </c>
       <c r="C413">
@@ -10260,7 +10257,7 @@
       <c r="A414">
         <v>426</v>
       </c>
-      <c r="B414" s="12" t="s">
+      <c r="B414" t="s">
         <v>2</v>
       </c>
       <c r="C414">
@@ -10272,7 +10269,7 @@
       <c r="A415">
         <v>428</v>
       </c>
-      <c r="B415" s="12" t="s">
+      <c r="B415" t="s">
         <v>0</v>
       </c>
       <c r="C415">
@@ -10284,7 +10281,7 @@
       <c r="A416">
         <v>431</v>
       </c>
-      <c r="B416" s="12" t="s">
+      <c r="B416" t="s">
         <v>2</v>
       </c>
       <c r="C416">
@@ -10296,7 +10293,7 @@
       <c r="A417">
         <v>433</v>
       </c>
-      <c r="B417" s="12" t="s">
+      <c r="B417" t="s">
         <v>0</v>
       </c>
       <c r="C417">
@@ -10308,7 +10305,7 @@
       <c r="A418">
         <v>435</v>
       </c>
-      <c r="B418" s="12" t="s">
+      <c r="B418" t="s">
         <v>0</v>
       </c>
       <c r="C418">
@@ -10320,7 +10317,7 @@
       <c r="A419">
         <v>436</v>
       </c>
-      <c r="B419" s="12" t="s">
+      <c r="B419" t="s">
         <v>3</v>
       </c>
       <c r="C419">
@@ -10332,7 +10329,7 @@
       <c r="A420">
         <v>438</v>
       </c>
-      <c r="B420" s="12" t="s">
+      <c r="B420" t="s">
         <v>0</v>
       </c>
       <c r="C420">
@@ -10344,7 +10341,7 @@
       <c r="A421">
         <v>439</v>
       </c>
-      <c r="B421" s="12" t="s">
+      <c r="B421" t="s">
         <v>0</v>
       </c>
       <c r="C421">
@@ -10356,7 +10353,7 @@
       <c r="A422">
         <v>440</v>
       </c>
-      <c r="B422" s="12" t="s">
+      <c r="B422" t="s">
         <v>0</v>
       </c>
       <c r="C422">
@@ -10368,7 +10365,7 @@
       <c r="A423">
         <v>441</v>
       </c>
-      <c r="B423" s="12" t="s">
+      <c r="B423" t="s">
         <v>2</v>
       </c>
       <c r="C423">
@@ -10380,7 +10377,7 @@
       <c r="A424">
         <v>442</v>
       </c>
-      <c r="B424" s="12" t="s">
+      <c r="B424" t="s">
         <v>0</v>
       </c>
       <c r="C424">
@@ -10392,7 +10389,7 @@
       <c r="A425">
         <v>443</v>
       </c>
-      <c r="B425" s="12" t="s">
+      <c r="B425" t="s">
         <v>1</v>
       </c>
       <c r="C425">
@@ -10404,7 +10401,7 @@
       <c r="A426">
         <v>444</v>
       </c>
-      <c r="B426" s="12" t="s">
+      <c r="B426" t="s">
         <v>5</v>
       </c>
       <c r="C426">
@@ -10416,7 +10413,7 @@
       <c r="A427">
         <v>446</v>
       </c>
-      <c r="B427" s="12" t="s">
+      <c r="B427" t="s">
         <v>0</v>
       </c>
       <c r="C427">
@@ -10428,7 +10425,7 @@
       <c r="A428">
         <v>448</v>
       </c>
-      <c r="B428" s="12" t="s">
+      <c r="B428" t="s">
         <v>0</v>
       </c>
       <c r="C428">
@@ -10440,7 +10437,7 @@
       <c r="A429">
         <v>449</v>
       </c>
-      <c r="B429" s="12" t="s">
+      <c r="B429" t="s">
         <v>2</v>
       </c>
       <c r="C429">
@@ -10452,7 +10449,7 @@
       <c r="A430">
         <v>451</v>
       </c>
-      <c r="B430" s="12" t="s">
+      <c r="B430" t="s">
         <v>0</v>
       </c>
       <c r="C430">
@@ -10464,7 +10461,7 @@
       <c r="A431">
         <v>457</v>
       </c>
-      <c r="B431" s="12" t="s">
+      <c r="B431" t="s">
         <v>0</v>
       </c>
       <c r="C431">
@@ -10476,7 +10473,7 @@
       <c r="A432">
         <v>467</v>
       </c>
-      <c r="B432" s="12" t="s">
+      <c r="B432" t="s">
         <v>1</v>
       </c>
       <c r="C432">
@@ -10488,7 +10485,7 @@
       <c r="A433">
         <v>469</v>
       </c>
-      <c r="B433" s="12" t="s">
+      <c r="B433" t="s">
         <v>0</v>
       </c>
       <c r="C433">
@@ -10500,7 +10497,7 @@
       <c r="A434">
         <v>475</v>
       </c>
-      <c r="B434" s="12" t="s">
+      <c r="B434" t="s">
         <v>1</v>
       </c>
       <c r="C434">
@@ -10512,7 +10509,7 @@
       <c r="A435">
         <v>503</v>
       </c>
-      <c r="B435" s="12" t="s">
+      <c r="B435" t="s">
         <v>0</v>
       </c>
       <c r="C435">
@@ -10524,7 +10521,7 @@
       <c r="A436">
         <v>506</v>
       </c>
-      <c r="B436" s="12" t="s">
+      <c r="B436" t="s">
         <v>0</v>
       </c>
       <c r="C436">
@@ -10536,7 +10533,7 @@
       <c r="A437">
         <v>508</v>
       </c>
-      <c r="B437" s="12" t="s">
+      <c r="B437" t="s">
         <v>0</v>
       </c>
       <c r="C437">
@@ -10548,7 +10545,7 @@
       <c r="A438">
         <v>524</v>
       </c>
-      <c r="B438" s="12" t="s">
+      <c r="B438" t="s">
         <v>0</v>
       </c>
       <c r="C438">
@@ -10570,8 +10567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A805777-2DE1-4985-9AED-C61B25849AA1}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10586,17 +10583,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="A1" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
@@ -10627,7 +10624,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3">
         <v>0.32993600000000001</v>
@@ -10656,7 +10653,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4">
         <v>0.32803700000000002</v>
@@ -10685,7 +10682,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5">
         <v>0.32795299999999999</v>
@@ -10714,7 +10711,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6">
         <v>0.33064700000000002</v>
@@ -10743,7 +10740,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B7">
         <v>0.33043400000000001</v>
@@ -10772,7 +10769,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8">
         <v>0.328706</v>
@@ -10801,7 +10798,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B9">
         <v>0.33099400000000001</v>
@@ -10830,7 +10827,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B10">
         <v>0.32828800000000002</v>
@@ -10859,7 +10856,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B11">
         <v>0.32941199999999998</v>
@@ -10888,7 +10885,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B12">
         <v>0.33097799999999999</v>
@@ -10953,17 +10950,17 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
+      <c r="A14" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
@@ -10994,7 +10991,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B16" s="5">
         <v>0.31323899999999999</v>
@@ -11023,7 +11020,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B17" s="6">
         <v>0.31436999999999998</v>
@@ -11052,7 +11049,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B18" s="5">
         <v>0.312587</v>
@@ -11081,7 +11078,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B19" s="6">
         <v>0.314052</v>
@@ -11110,7 +11107,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B20" s="5">
         <v>0.31265599999999999</v>
@@ -11139,7 +11136,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B21" s="6">
         <v>0.31306299999999998</v>
@@ -11168,7 +11165,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B22" s="5">
         <v>0.31348599999999999</v>
@@ -11197,7 +11194,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B23" s="6">
         <v>0.31276700000000002</v>
@@ -11226,7 +11223,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B24" s="5">
         <v>0.31517699999999998</v>
@@ -11255,7 +11252,7 @@
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B25" s="6">
         <v>0.31365399999999999</v>

</xml_diff>